<commit_message>
Switch to colemak and combo mods, new branch.
</commit_message>
<xml_diff>
--- a/Urchin Layouts.xlsx
+++ b/Urchin Layouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhsch\Documents\Development\zmk-urchin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F12F426E-39B9-4BD9-97A9-A5A6E62E0A93}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CFC754-70D4-4D74-B607-370F24EA6222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15945" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="101">
   <si>
     <t>esc</t>
   </si>
@@ -266,12 +266,6 @@
     <t>caps</t>
   </si>
   <si>
-    <t>tab</t>
-  </si>
-  <si>
-    <t>spc</t>
-  </si>
-  <si>
     <t>ent</t>
   </si>
   <si>
@@ -284,42 +278,9 @@
     <t>pg dn</t>
   </si>
   <si>
-    <t>m↑</t>
-  </si>
-  <si>
-    <t>m↓</t>
-  </si>
-  <si>
-    <t>m→</t>
-  </si>
-  <si>
-    <t>←m</t>
-  </si>
-  <si>
     <t>num</t>
   </si>
   <si>
-    <t>m1</t>
-  </si>
-  <si>
-    <t>m2</t>
-  </si>
-  <si>
-    <t>m up</t>
-  </si>
-  <si>
-    <t>m dn</t>
-  </si>
-  <si>
-    <t>m wl</t>
-  </si>
-  <si>
-    <t>m wr</t>
-  </si>
-  <si>
-    <t>m3</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 0 Base</t>
   </si>
   <si>
@@ -327,9 +288,6 @@
   </si>
   <si>
     <t>2 Symbol</t>
-  </si>
-  <si>
-    <t>3 Mirror</t>
   </si>
   <si>
     <t>4 Number</t>
@@ -364,6 +322,24 @@
   </si>
   <si>
     <t>USTK</t>
+  </si>
+  <si>
+    <t>shift</t>
+  </si>
+  <si>
+    <t>gui</t>
+  </si>
+  <si>
+    <t>alt</t>
+  </si>
+  <si>
+    <t>ctrl</t>
+  </si>
+  <si>
+    <t>spc</t>
+  </si>
+  <si>
+    <t>tab</t>
   </si>
 </sst>
 </file>
@@ -716,7 +692,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="52">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -730,9 +706,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="17" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -826,9 +799,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -857,9 +827,22 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1206,7 +1189,7 @@
   <dimension ref="B2:AP18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Z2" sqref="B2:AJ12"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1215,686 +1198,626 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="48" t="s">
-        <v>94</v>
-      </c>
-      <c r="C2" s="48"/>
-      <c r="D2" s="48"/>
-      <c r="E2" s="48"/>
-      <c r="F2" s="48"/>
-      <c r="G2" s="48"/>
-      <c r="H2" s="48"/>
-      <c r="I2" s="48"/>
-      <c r="J2" s="48"/>
-      <c r="K2" s="48"/>
-      <c r="L2" s="48"/>
-      <c r="N2" s="48" t="s">
-        <v>95</v>
-      </c>
-      <c r="O2" s="48"/>
-      <c r="P2" s="48"/>
-      <c r="Q2" s="48"/>
-      <c r="R2" s="48"/>
-      <c r="S2" s="48"/>
-      <c r="T2" s="48"/>
-      <c r="U2" s="48"/>
-      <c r="V2" s="48"/>
-      <c r="W2" s="48"/>
-      <c r="X2" s="48"/>
-      <c r="Z2" s="48" t="s">
-        <v>96</v>
-      </c>
-      <c r="AA2" s="48"/>
-      <c r="AB2" s="48"/>
-      <c r="AC2" s="48"/>
-      <c r="AD2" s="48"/>
-      <c r="AE2" s="48"/>
-      <c r="AF2" s="48"/>
-      <c r="AG2" s="48"/>
-      <c r="AH2" s="48"/>
-      <c r="AI2" s="48"/>
-      <c r="AJ2" s="48"/>
+      <c r="B2" s="50" t="s">
+        <v>81</v>
+      </c>
+      <c r="C2" s="50"/>
+      <c r="D2" s="50"/>
+      <c r="E2" s="50"/>
+      <c r="F2" s="50"/>
+      <c r="G2" s="50"/>
+      <c r="H2" s="50"/>
+      <c r="I2" s="50"/>
+      <c r="J2" s="50"/>
+      <c r="K2" s="50"/>
+      <c r="L2" s="50"/>
+      <c r="N2" s="50" t="s">
+        <v>82</v>
+      </c>
+      <c r="O2" s="50"/>
+      <c r="P2" s="50"/>
+      <c r="Q2" s="50"/>
+      <c r="R2" s="50"/>
+      <c r="S2" s="50"/>
+      <c r="T2" s="50"/>
+      <c r="U2" s="50"/>
+      <c r="V2" s="50"/>
+      <c r="W2" s="50"/>
+      <c r="X2" s="50"/>
+      <c r="Z2" s="50" t="s">
+        <v>83</v>
+      </c>
+      <c r="AA2" s="50"/>
+      <c r="AB2" s="50"/>
+      <c r="AC2" s="50"/>
+      <c r="AD2" s="50"/>
+      <c r="AE2" s="50"/>
+      <c r="AF2" s="50"/>
+      <c r="AG2" s="50"/>
+      <c r="AH2" s="50"/>
+      <c r="AI2" s="50"/>
+      <c r="AJ2" s="50"/>
     </row>
     <row r="3" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="7" t="s">
+      <c r="C3" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="E3" s="7" t="s">
-        <v>35</v>
-      </c>
-      <c r="F3" s="9" t="s">
-        <v>36</v>
-      </c>
-      <c r="G3" s="10"/>
-      <c r="H3" s="6" t="s">
+      <c r="D3" s="7" t="s">
+        <v>45</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="F3" s="8" t="s">
+        <v>55</v>
+      </c>
+      <c r="G3" s="9"/>
+      <c r="H3" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="I3" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>38</v>
+      </c>
+      <c r="K3" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="I3" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="J3" s="7" t="s">
-        <v>39</v>
-      </c>
-      <c r="K3" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>41</v>
-      </c>
-      <c r="N3" s="6"/>
-      <c r="O3" s="26" t="s">
-        <v>88</v>
-      </c>
-      <c r="P3" s="27" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q3" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="R3" s="9" t="s">
-        <v>89</v>
-      </c>
-      <c r="S3" s="10"/>
-      <c r="T3" s="6" t="s">
+      <c r="L3" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="N3" s="5"/>
+      <c r="O3" s="25"/>
+      <c r="P3" s="26"/>
+      <c r="Q3" s="25"/>
+      <c r="R3" s="8"/>
+      <c r="S3" s="9"/>
+      <c r="T3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="U3" s="26" t="s">
-        <v>80</v>
-      </c>
-      <c r="V3" s="27" t="s">
+      <c r="U3" s="25" t="s">
+        <v>78</v>
+      </c>
+      <c r="V3" s="26" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="26" t="s">
+      <c r="W3" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="X3" s="9" t="s">
+      <c r="X3" s="8" t="s">
         <v>0</v>
       </c>
-      <c r="Z3" s="6" t="s">
+      <c r="Z3" s="5" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="7" t="s">
+      <c r="AA3" s="6" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="36" t="s">
+      <c r="AB3" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="AC3" s="7" t="s">
+      <c r="AC3" s="6" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="25" t="s">
+      <c r="AD3" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="AE3" s="10"/>
-      <c r="AF3" s="6"/>
-      <c r="AG3" s="7" t="s">
+      <c r="AE3" s="9"/>
+      <c r="AF3" s="5"/>
+      <c r="AG3" s="6" t="s">
         <v>27</v>
       </c>
-      <c r="AH3" s="7" t="s">
+      <c r="AH3" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="AI3" s="7" t="s">
+      <c r="AI3" s="6" t="s">
         <v>17</v>
       </c>
-      <c r="AJ3" s="9" t="s">
+      <c r="AJ3" s="8" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="11" t="s">
+      <c r="B4" s="10" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="11" t="s">
+        <v>35</v>
+      </c>
+      <c r="D4" s="12" t="s">
         <v>43</v>
       </c>
-      <c r="D4" s="13" t="s">
-        <v>44</v>
-      </c>
-      <c r="E4" s="12" t="s">
-        <v>45</v>
-      </c>
-      <c r="F4" s="14" t="s">
+      <c r="E4" s="11" t="s">
+        <v>36</v>
+      </c>
+      <c r="F4" s="13" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="10"/>
-      <c r="H4" s="11" t="s">
-        <v>47</v>
-      </c>
-      <c r="I4" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="J4" s="12" t="s">
-        <v>49</v>
-      </c>
-      <c r="K4" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="L4" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="N4" s="11"/>
-      <c r="O4" s="29" t="s">
-        <v>85</v>
-      </c>
-      <c r="P4" s="29" t="s">
-        <v>83</v>
-      </c>
-      <c r="Q4" s="29" t="s">
-        <v>84</v>
-      </c>
-      <c r="R4" s="14" t="s">
-        <v>93</v>
-      </c>
-      <c r="S4" s="10"/>
-      <c r="T4" s="30" t="s">
+      <c r="G4" s="9"/>
+      <c r="H4" s="10" t="s">
+        <v>57</v>
+      </c>
+      <c r="I4" s="11" t="s">
+        <v>56</v>
+      </c>
+      <c r="J4" s="11" t="s">
+        <v>34</v>
+      </c>
+      <c r="K4" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="L4" s="13" t="s">
+        <v>40</v>
+      </c>
+      <c r="N4" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="O4" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="P4" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="Q4" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="R4" s="13"/>
+      <c r="S4" s="9"/>
+      <c r="T4" s="29" t="s">
         <v>73</v>
       </c>
-      <c r="U4" s="29" t="s">
+      <c r="U4" s="28" t="s">
         <v>9</v>
       </c>
-      <c r="V4" s="29" t="s">
+      <c r="V4" s="28" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="29" t="s">
+      <c r="W4" s="28" t="s">
         <v>6</v>
       </c>
-      <c r="X4" s="31" t="s">
+      <c r="X4" s="30" t="s">
         <v>74</v>
       </c>
-      <c r="Z4" s="11" t="s">
+      <c r="Z4" s="10" t="s">
         <v>21</v>
       </c>
-      <c r="AA4" s="12" t="s">
+      <c r="AA4" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="AB4" s="13" t="s">
+      <c r="AB4" s="12" t="s">
         <v>19</v>
       </c>
-      <c r="AC4" s="12" t="s">
+      <c r="AC4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="AD4" s="28" t="s">
+      <c r="AD4" s="27" t="s">
         <v>70</v>
       </c>
-      <c r="AE4" s="10"/>
-      <c r="AF4" s="11" t="s">
+      <c r="AE4" s="9"/>
+      <c r="AF4" s="10" t="s">
         <v>31</v>
       </c>
-      <c r="AG4" s="38" t="s">
+      <c r="AG4" s="36" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" s="12" t="s">
+      <c r="AH4" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="AI4" s="12" t="s">
+      <c r="AI4" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="AJ4" s="14" t="s">
+      <c r="AJ4" s="13" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="15" t="s">
+      <c r="B5" s="14" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="16" t="s">
+      <c r="C5" s="15" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="17" t="s">
+      <c r="D5" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="12" t="s">
+      <c r="E5" s="11" t="s">
+        <v>44</v>
+      </c>
+      <c r="F5" s="12" t="s">
         <v>53</v>
       </c>
-      <c r="F5" s="13" t="s">
-        <v>55</v>
-      </c>
-      <c r="G5" s="18"/>
-      <c r="H5" s="11" t="s">
-        <v>56</v>
-      </c>
-      <c r="I5" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="J5" s="16" t="s">
+      <c r="G5" s="17"/>
+      <c r="H5" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="I5" s="11" t="s">
+        <v>47</v>
+      </c>
+      <c r="J5" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="16" t="s">
+      <c r="K5" s="15" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="19" t="s">
+      <c r="L5" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="15"/>
-      <c r="O5" s="16" t="s">
-        <v>91</v>
-      </c>
-      <c r="P5" s="17" t="s">
-        <v>92</v>
-      </c>
-      <c r="Q5" s="12"/>
-      <c r="R5" s="13" t="s">
-        <v>90</v>
-      </c>
-      <c r="S5" s="18"/>
-      <c r="T5" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="U5" s="33" t="s">
-        <v>81</v>
-      </c>
-      <c r="V5" s="34" t="s">
+      <c r="N5" s="14"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="16"/>
+      <c r="Q5" s="11"/>
+      <c r="R5" s="12"/>
+      <c r="S5" s="17"/>
+      <c r="T5" s="10" t="s">
+        <v>80</v>
+      </c>
+      <c r="U5" s="32" t="s">
         <v>79</v>
       </c>
-      <c r="W5" s="34" t="s">
+      <c r="V5" s="33" t="s">
+        <v>77</v>
+      </c>
+      <c r="W5" s="33" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="19"/>
-      <c r="Z5" s="15" t="s">
+      <c r="X5" s="18"/>
+      <c r="Z5" s="14" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="16" t="s">
+      <c r="AA5" s="15" t="s">
         <v>25</v>
       </c>
-      <c r="AB5" s="40" t="s">
+      <c r="AB5" s="38" t="s">
         <v>24</v>
       </c>
-      <c r="AC5" s="12" t="s">
+      <c r="AC5" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="AD5" s="32" t="s">
+      <c r="AD5" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="AE5" s="18"/>
-      <c r="AF5" s="11"/>
-      <c r="AG5" s="12" t="s">
+      <c r="AE5" s="17"/>
+      <c r="AF5" s="10"/>
+      <c r="AG5" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="AH5" s="16" t="s">
+      <c r="AH5" s="15" t="s">
         <v>70</v>
       </c>
-      <c r="AI5" s="16" t="s">
+      <c r="AI5" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="AJ5" s="19" t="s">
+      <c r="AJ5" s="18" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="15" t="s">
+      <c r="B6" s="9"/>
+      <c r="C6" s="9"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="47" t="s">
+        <v>100</v>
+      </c>
+      <c r="F6" s="46" t="s">
+        <v>99</v>
+      </c>
+      <c r="G6" s="17"/>
+      <c r="H6" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="F6" s="21" t="s">
+      <c r="I6" s="47" t="s">
         <v>77</v>
       </c>
-      <c r="G6" s="18"/>
-      <c r="H6" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="I6" s="23" t="s">
-        <v>79</v>
-      </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="10"/>
-      <c r="P6" s="20"/>
-      <c r="Q6" s="15"/>
-      <c r="R6" s="21"/>
-      <c r="S6" s="18"/>
+      <c r="J6" s="9"/>
+      <c r="K6" s="9"/>
+      <c r="L6" s="9"/>
+      <c r="N6" s="9"/>
+      <c r="O6" s="9"/>
+      <c r="P6" s="19"/>
+      <c r="Q6" s="14"/>
+      <c r="R6" s="20"/>
+      <c r="S6" s="17"/>
       <c r="T6" s="4"/>
-      <c r="U6" s="23"/>
-      <c r="V6" s="10"/>
-      <c r="W6" s="10"/>
-      <c r="X6" s="10"/>
-      <c r="Z6" s="10"/>
-      <c r="AA6" s="10"/>
-      <c r="AB6" s="20"/>
-      <c r="AC6" s="15"/>
-      <c r="AD6" s="21"/>
-      <c r="AE6" s="18"/>
-      <c r="AF6" s="22"/>
-      <c r="AG6" s="5"/>
-      <c r="AH6" s="10"/>
-      <c r="AI6" s="10"/>
-      <c r="AJ6" s="10"/>
+      <c r="U6" s="22"/>
+      <c r="V6" s="9"/>
+      <c r="W6" s="9"/>
+      <c r="X6" s="9"/>
+      <c r="Z6" s="9"/>
+      <c r="AA6" s="9"/>
+      <c r="AB6" s="19"/>
+      <c r="AC6" s="2"/>
+      <c r="AD6" s="20"/>
+      <c r="AE6" s="17"/>
+      <c r="AF6" s="21"/>
+      <c r="AG6" s="20"/>
+      <c r="AH6" s="9"/>
+      <c r="AI6" s="9"/>
+      <c r="AJ6" s="9"/>
     </row>
     <row r="7" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="24"/>
+      <c r="E7" s="23"/>
     </row>
     <row r="8" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="48" t="s">
-        <v>99</v>
-      </c>
-      <c r="C8" s="48"/>
-      <c r="D8" s="48"/>
-      <c r="E8" s="48"/>
-      <c r="F8" s="48"/>
-      <c r="G8" s="48"/>
-      <c r="H8" s="48"/>
-      <c r="I8" s="48"/>
-      <c r="J8" s="48"/>
-      <c r="K8" s="48"/>
-      <c r="L8" s="48"/>
-      <c r="N8" s="48" t="s">
-        <v>98</v>
-      </c>
-      <c r="O8" s="48"/>
-      <c r="P8" s="48"/>
-      <c r="Q8" s="48"/>
-      <c r="R8" s="48"/>
-      <c r="S8" s="48"/>
-      <c r="T8" s="48"/>
-      <c r="U8" s="48"/>
-      <c r="V8" s="48"/>
-      <c r="W8" s="48"/>
-      <c r="X8" s="48"/>
-      <c r="Z8" s="48" t="s">
-        <v>97</v>
-      </c>
-      <c r="AA8" s="48"/>
-      <c r="AB8" s="48"/>
-      <c r="AC8" s="48"/>
-      <c r="AD8" s="48"/>
-      <c r="AE8" s="48"/>
-      <c r="AF8" s="48"/>
-      <c r="AG8" s="48"/>
-      <c r="AH8" s="48"/>
-      <c r="AI8" s="48"/>
-      <c r="AJ8" s="48"/>
+      <c r="B8" s="50" t="s">
+        <v>85</v>
+      </c>
+      <c r="C8" s="50"/>
+      <c r="D8" s="50"/>
+      <c r="E8" s="50"/>
+      <c r="F8" s="50"/>
+      <c r="G8" s="50"/>
+      <c r="H8" s="50"/>
+      <c r="I8" s="50"/>
+      <c r="J8" s="50"/>
+      <c r="K8" s="50"/>
+      <c r="L8" s="50"/>
+      <c r="N8" s="50" t="s">
+        <v>84</v>
+      </c>
+      <c r="O8" s="50"/>
+      <c r="P8" s="50"/>
+      <c r="Q8" s="50"/>
+      <c r="R8" s="50"/>
+      <c r="S8" s="50"/>
+      <c r="T8" s="50"/>
+      <c r="U8" s="50"/>
+      <c r="V8" s="50"/>
+      <c r="W8" s="50"/>
+      <c r="X8" s="50"/>
+      <c r="Z8" s="51"/>
+      <c r="AA8" s="51"/>
+      <c r="AB8" s="51"/>
+      <c r="AC8" s="51"/>
+      <c r="AD8" s="51"/>
+      <c r="AE8" s="51"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
     </row>
     <row r="9" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7" t="s">
-        <v>100</v>
-      </c>
-      <c r="F9" s="9" t="s">
-        <v>104</v>
-      </c>
-      <c r="G9" s="10"/>
-      <c r="H9" s="6"/>
-      <c r="I9" s="7"/>
-      <c r="J9" s="7"/>
-      <c r="K9" s="7"/>
-      <c r="L9" s="9"/>
-      <c r="N9" s="35" t="s">
+      <c r="B9" s="49" t="s">
+        <v>89</v>
+      </c>
+      <c r="C9" s="6"/>
+      <c r="D9" s="7"/>
+      <c r="E9" s="6"/>
+      <c r="F9" s="8" t="s">
+        <v>86</v>
+      </c>
+      <c r="G9" s="9"/>
+      <c r="H9" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="I9" s="6"/>
+      <c r="J9" s="6"/>
+      <c r="K9" s="6"/>
+      <c r="L9" s="48" t="s">
+        <v>89</v>
+      </c>
+      <c r="N9" s="34" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="41" t="s">
+      <c r="O9" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="P9" s="36" t="s">
+      <c r="P9" s="35" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="41" t="s">
+      <c r="Q9" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="R9" s="25" t="s">
+      <c r="R9" s="24" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="10"/>
-      <c r="T9" s="6"/>
-      <c r="U9" s="7" t="s">
+      <c r="S9" s="9"/>
+      <c r="T9" s="5"/>
+      <c r="U9" s="6" t="s">
         <v>68</v>
       </c>
-      <c r="V9" s="7" t="s">
+      <c r="V9" s="6" t="s">
         <v>69</v>
       </c>
-      <c r="W9" s="7"/>
-      <c r="X9" s="9"/>
-      <c r="Z9" s="6" t="s">
-        <v>41</v>
-      </c>
-      <c r="AA9" s="7" t="s">
-        <v>40</v>
-      </c>
-      <c r="AB9" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="AC9" s="7" t="s">
-        <v>38</v>
-      </c>
-      <c r="AD9" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="AE9" s="10"/>
-      <c r="AF9" s="35" t="s">
-        <v>30</v>
-      </c>
-      <c r="AG9" s="7">
-        <v>7</v>
-      </c>
-      <c r="AH9" s="7">
-        <v>8</v>
-      </c>
-      <c r="AI9" s="7">
-        <v>9</v>
-      </c>
-      <c r="AJ9" s="9">
-        <v>0</v>
-      </c>
+      <c r="W9" s="6"/>
+      <c r="X9" s="8"/>
+      <c r="Z9"/>
+      <c r="AA9"/>
+      <c r="AB9"/>
+      <c r="AC9"/>
+      <c r="AD9"/>
+      <c r="AE9"/>
+      <c r="AF9" s="40"/>
+      <c r="AG9"/>
+      <c r="AH9"/>
+      <c r="AI9"/>
+      <c r="AJ9"/>
     </row>
     <row r="10" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="11"/>
-      <c r="C10" s="12"/>
-      <c r="D10" s="45" t="s">
-        <v>103</v>
-      </c>
-      <c r="E10" s="12" t="s">
-        <v>101</v>
-      </c>
-      <c r="F10" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="G10" s="10"/>
-      <c r="H10" s="11"/>
-      <c r="I10" s="12"/>
-      <c r="J10" s="12"/>
-      <c r="K10" s="12"/>
-      <c r="L10" s="14"/>
-      <c r="N10" s="11">
+      <c r="B10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="D10" s="43" t="s">
+        <v>95</v>
+      </c>
+      <c r="E10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="F10" s="13" t="s">
+        <v>87</v>
+      </c>
+      <c r="G10" s="9"/>
+      <c r="H10" s="10" t="s">
+        <v>91</v>
+      </c>
+      <c r="I10" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="J10" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="K10" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="L10" s="13" t="s">
+        <v>96</v>
+      </c>
+      <c r="N10" s="10">
         <v>4</v>
       </c>
-      <c r="O10" s="12">
+      <c r="O10" s="11">
         <v>3</v>
       </c>
-      <c r="P10" s="13">
+      <c r="P10" s="12">
         <v>2</v>
       </c>
-      <c r="Q10" s="12">
+      <c r="Q10" s="11">
         <v>1</v>
       </c>
-      <c r="R10" s="28">
+      <c r="R10" s="27">
         <v>0</v>
       </c>
-      <c r="S10" s="10"/>
-      <c r="T10" s="11" t="s">
+      <c r="S10" s="9"/>
+      <c r="T10" s="10" t="s">
         <v>67</v>
       </c>
-      <c r="U10" s="12" t="s">
+      <c r="U10" s="11" t="s">
         <v>58</v>
       </c>
-      <c r="V10" s="12" t="s">
+      <c r="V10" s="11" t="s">
         <v>59</v>
       </c>
-      <c r="W10" s="12" t="s">
+      <c r="W10" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="X10" s="14" t="s">
+      <c r="X10" s="13" t="s">
         <v>61</v>
       </c>
-      <c r="Z10" s="11" t="s">
-        <v>1</v>
-      </c>
-      <c r="AA10" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="AB10" s="13" t="s">
-        <v>49</v>
-      </c>
-      <c r="AC10" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="AD10" s="14" t="s">
-        <v>47</v>
-      </c>
-      <c r="AE10" s="10"/>
-      <c r="AF10" s="37" t="s">
-        <v>15</v>
-      </c>
-      <c r="AG10" s="12">
-        <v>4</v>
-      </c>
-      <c r="AH10" s="12">
-        <v>5</v>
-      </c>
-      <c r="AI10" s="12">
-        <v>6</v>
-      </c>
-      <c r="AJ10" s="14" t="s">
-        <v>4</v>
-      </c>
+      <c r="Z10"/>
+      <c r="AA10"/>
+      <c r="AB10"/>
+      <c r="AC10"/>
+      <c r="AD10"/>
+      <c r="AE10"/>
+      <c r="AF10" s="40"/>
+      <c r="AG10"/>
+      <c r="AH10"/>
+      <c r="AI10"/>
+      <c r="AJ10"/>
     </row>
     <row r="11" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="39" t="s">
-        <v>107</v>
-      </c>
-      <c r="C11" s="16"/>
-      <c r="D11" s="17"/>
-      <c r="E11" s="12" t="s">
-        <v>102</v>
-      </c>
-      <c r="F11" s="13" t="s">
-        <v>106</v>
-      </c>
-      <c r="G11" s="18"/>
-      <c r="H11" s="11"/>
-      <c r="I11" s="12"/>
-      <c r="J11" s="12"/>
-      <c r="K11" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="L11" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="N11" s="15">
+      <c r="B11" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" s="15"/>
+      <c r="D11" s="16"/>
+      <c r="E11" s="11"/>
+      <c r="F11" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="G11" s="17"/>
+      <c r="H11" s="10" t="s">
+        <v>92</v>
+      </c>
+      <c r="I11" s="11"/>
+      <c r="J11" s="11"/>
+      <c r="K11" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="L11" s="13" t="s">
+        <v>93</v>
+      </c>
+      <c r="N11" s="14">
         <v>9</v>
       </c>
-      <c r="O11" s="16">
+      <c r="O11" s="15">
         <v>8</v>
       </c>
-      <c r="P11" s="17">
+      <c r="P11" s="16">
         <v>7</v>
       </c>
-      <c r="Q11" s="12">
+      <c r="Q11" s="11">
         <v>6</v>
       </c>
-      <c r="R11" s="32">
+      <c r="R11" s="31">
         <v>5</v>
       </c>
-      <c r="S11" s="18"/>
-      <c r="T11" s="11" t="s">
+      <c r="S11" s="17"/>
+      <c r="T11" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="U11" s="12" t="s">
+      <c r="U11" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="V11" s="16" t="s">
+      <c r="V11" s="15" t="s">
         <v>64</v>
       </c>
-      <c r="W11" s="16" t="s">
+      <c r="W11" s="15" t="s">
         <v>65</v>
       </c>
-      <c r="X11" s="19" t="s">
+      <c r="X11" s="18" t="s">
         <v>66</v>
       </c>
-      <c r="Z11" s="39" t="s">
-        <v>2</v>
-      </c>
-      <c r="AA11" s="16" t="s">
-        <v>4</v>
-      </c>
-      <c r="AB11" s="17" t="s">
-        <v>5</v>
-      </c>
-      <c r="AC11" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="AD11" s="13" t="s">
-        <v>56</v>
-      </c>
-      <c r="AE11" s="18"/>
-      <c r="AF11" s="37" t="s">
-        <v>14</v>
-      </c>
-      <c r="AG11" s="12">
-        <v>1</v>
-      </c>
-      <c r="AH11" s="16">
-        <v>2</v>
-      </c>
-      <c r="AI11" s="16">
-        <v>3</v>
-      </c>
-      <c r="AJ11" s="19" t="s">
-        <v>25</v>
-      </c>
+      <c r="Z11" s="40"/>
+      <c r="AA11"/>
+      <c r="AB11"/>
+      <c r="AC11"/>
+      <c r="AD11"/>
+      <c r="AE11"/>
+      <c r="AF11" s="40"/>
+      <c r="AG11"/>
+      <c r="AH11"/>
+      <c r="AI11"/>
+      <c r="AJ11" s="40"/>
     </row>
     <row r="12" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="10"/>
-      <c r="C12" s="10"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="43"/>
-      <c r="F12" s="44"/>
-      <c r="G12" s="18"/>
-      <c r="H12" s="46"/>
-      <c r="I12" s="47"/>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="10"/>
-      <c r="P12" s="20"/>
-      <c r="Q12" s="15"/>
+      <c r="B12" s="9"/>
+      <c r="C12" s="9"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="42"/>
+      <c r="G12" s="17"/>
+      <c r="H12" s="44"/>
+      <c r="I12" s="45"/>
+      <c r="J12" s="9"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="9"/>
+      <c r="N12" s="9"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="19"/>
+      <c r="Q12" s="14"/>
       <c r="R12" s="3"/>
-      <c r="S12" s="18"/>
-      <c r="T12" s="22"/>
-      <c r="U12" s="23"/>
-      <c r="V12" s="10"/>
-      <c r="W12" s="10"/>
-      <c r="X12" s="10"/>
-      <c r="Z12" s="10"/>
-      <c r="AA12" s="10"/>
-      <c r="AB12" s="20"/>
-      <c r="AC12" s="2"/>
-      <c r="AD12" s="21"/>
-      <c r="AE12" s="18"/>
-      <c r="AF12" s="22" t="s">
-        <v>78</v>
-      </c>
-      <c r="AG12" s="23"/>
-      <c r="AH12" s="10"/>
-      <c r="AI12" s="10"/>
-      <c r="AJ12" s="10"/>
+      <c r="S12" s="17"/>
+      <c r="T12" s="21"/>
+      <c r="U12" s="22"/>
+      <c r="V12" s="9"/>
+      <c r="W12" s="9"/>
+      <c r="X12" s="9"/>
+      <c r="Z12"/>
+      <c r="AA12"/>
+      <c r="AB12"/>
+      <c r="AC12"/>
+      <c r="AD12"/>
+      <c r="AE12"/>
+      <c r="AF12"/>
+      <c r="AG12"/>
+      <c r="AH12"/>
+      <c r="AI12"/>
+      <c r="AJ12"/>
     </row>
     <row r="14" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z14"/>
       <c r="AA14"/>
-      <c r="AB14" s="42"/>
+      <c r="AB14" s="40"/>
       <c r="AC14"/>
-      <c r="AD14" s="42"/>
+      <c r="AD14" s="40"/>
       <c r="AK14"/>
       <c r="AL14"/>
       <c r="AM14"/>
@@ -1907,7 +1830,7 @@
       <c r="AA15"/>
       <c r="AB15"/>
       <c r="AC15"/>
-      <c r="AD15" s="42"/>
+      <c r="AD15" s="40"/>
       <c r="AK15"/>
       <c r="AL15"/>
       <c r="AM15"/>
@@ -1918,9 +1841,9 @@
     <row r="16" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z16"/>
       <c r="AA16"/>
-      <c r="AB16" s="42"/>
+      <c r="AB16" s="40"/>
       <c r="AC16"/>
-      <c r="AD16" s="42"/>
+      <c r="AD16" s="40"/>
       <c r="AK16"/>
       <c r="AL16"/>
       <c r="AM16"/>

</xml_diff>

<commit_message>
Change to 2 key combos, added function layer, put mods more places
</commit_message>
<xml_diff>
--- a/Urchin Layouts.xlsx
+++ b/Urchin Layouts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhsch\Documents\Development\zmk-urchin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46CFC754-70D4-4D74-B607-370F24EA6222}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D1C401-1B70-4890-AAC9-B9DFC8F481DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="14610" windowHeight="15945" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
+    <workbookView xWindow="-105" yWindow="0" windowWidth="9975" windowHeight="15585" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="9" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="121" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
   <si>
     <t>esc</t>
   </si>
@@ -291,9 +291,6 @@
   </si>
   <si>
     <t>4 Number</t>
-  </si>
-  <si>
-    <t>5 Settings</t>
   </si>
   <si>
     <t>BT0</t>
@@ -340,6 +337,57 @@
   </si>
   <si>
     <t>tab</t>
+  </si>
+  <si>
+    <t>A+R</t>
+  </si>
+  <si>
+    <t>6 Settings</t>
+  </si>
+  <si>
+    <t>5 Function</t>
+  </si>
+  <si>
+    <t>cut</t>
+  </si>
+  <si>
+    <t>undo</t>
+  </si>
+  <si>
+    <t>copy</t>
+  </si>
+  <si>
+    <t>paste</t>
+  </si>
+  <si>
+    <t>Combos</t>
+  </si>
+  <si>
+    <t>S+T</t>
+  </si>
+  <si>
+    <t>N+E</t>
+  </si>
+  <si>
+    <t>R+S</t>
+  </si>
+  <si>
+    <t>E+I</t>
+  </si>
+  <si>
+    <t>I+O</t>
+  </si>
+  <si>
+    <t>A+R+S+T</t>
+  </si>
+  <si>
+    <t>N+E+I+O</t>
+  </si>
+  <si>
+    <t>CAPS_WORD</t>
+  </si>
+  <si>
+    <t>S+E</t>
   </si>
 </sst>
 </file>
@@ -369,7 +417,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -394,6 +442,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="22">
     <border>
@@ -697,9 +751,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -842,7 +893,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1186,10 +1242,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:AP18"/>
+  <dimension ref="B2:AP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="R19" sqref="R19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1198,626 +1254,652 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="49" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
-      <c r="F2" s="50"/>
-      <c r="G2" s="50"/>
-      <c r="H2" s="50"/>
-      <c r="I2" s="50"/>
-      <c r="J2" s="50"/>
-      <c r="K2" s="50"/>
-      <c r="L2" s="50"/>
-      <c r="N2" s="50" t="s">
+      <c r="C2" s="49"/>
+      <c r="D2" s="49"/>
+      <c r="E2" s="49"/>
+      <c r="F2" s="49"/>
+      <c r="G2" s="49"/>
+      <c r="H2" s="49"/>
+      <c r="I2" s="49"/>
+      <c r="J2" s="49"/>
+      <c r="K2" s="49"/>
+      <c r="L2" s="49"/>
+      <c r="N2" s="49" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="50"/>
-      <c r="P2" s="50"/>
-      <c r="Q2" s="50"/>
-      <c r="R2" s="50"/>
-      <c r="S2" s="50"/>
-      <c r="T2" s="50"/>
-      <c r="U2" s="50"/>
-      <c r="V2" s="50"/>
-      <c r="W2" s="50"/>
-      <c r="X2" s="50"/>
-      <c r="Z2" s="50" t="s">
+      <c r="O2" s="49"/>
+      <c r="P2" s="49"/>
+      <c r="Q2" s="49"/>
+      <c r="R2" s="49"/>
+      <c r="S2" s="49"/>
+      <c r="T2" s="49"/>
+      <c r="U2" s="49"/>
+      <c r="V2" s="49"/>
+      <c r="W2" s="49"/>
+      <c r="X2" s="49"/>
+      <c r="Z2" s="49" t="s">
         <v>83</v>
       </c>
-      <c r="AA2" s="50"/>
-      <c r="AB2" s="50"/>
-      <c r="AC2" s="50"/>
-      <c r="AD2" s="50"/>
-      <c r="AE2" s="50"/>
-      <c r="AF2" s="50"/>
-      <c r="AG2" s="50"/>
-      <c r="AH2" s="50"/>
-      <c r="AI2" s="50"/>
-      <c r="AJ2" s="50"/>
+      <c r="AA2" s="49"/>
+      <c r="AB2" s="49"/>
+      <c r="AC2" s="49"/>
+      <c r="AD2" s="49"/>
+      <c r="AE2" s="49"/>
+      <c r="AF2" s="49"/>
+      <c r="AG2" s="49"/>
+      <c r="AH2" s="49"/>
+      <c r="AI2" s="49"/>
+      <c r="AJ2" s="49"/>
     </row>
     <row r="3" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="5" t="s">
+      <c r="B3" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>33</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="F3" s="8" t="s">
+      <c r="F3" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="G3" s="9"/>
-      <c r="H3" s="5" t="s">
+      <c r="G3" s="8"/>
+      <c r="H3" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="I3" s="6" t="s">
+      <c r="I3" s="5" t="s">
         <v>50</v>
       </c>
-      <c r="J3" s="6" t="s">
+      <c r="J3" s="5" t="s">
         <v>38</v>
       </c>
-      <c r="K3" s="6" t="s">
+      <c r="K3" s="5" t="s">
         <v>37</v>
       </c>
-      <c r="L3" s="8" t="s">
+      <c r="L3" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="5"/>
-      <c r="O3" s="25"/>
-      <c r="P3" s="26"/>
-      <c r="Q3" s="25"/>
-      <c r="R3" s="8"/>
-      <c r="S3" s="9"/>
-      <c r="T3" s="5" t="s">
+      <c r="N3" s="4"/>
+      <c r="O3" s="24"/>
+      <c r="P3" s="25"/>
+      <c r="Q3" s="24"/>
+      <c r="R3" s="7"/>
+      <c r="S3" s="8"/>
+      <c r="T3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="U3" s="25" t="s">
+      <c r="U3" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="V3" s="26" t="s">
+      <c r="V3" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="W3" s="25" t="s">
+      <c r="W3" s="24" t="s">
         <v>72</v>
       </c>
-      <c r="X3" s="8" t="s">
+      <c r="X3" s="7" t="s">
         <v>0</v>
       </c>
-      <c r="Z3" s="5" t="s">
+      <c r="Z3" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="AA3" s="6" t="s">
+      <c r="AA3" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="AB3" s="35" t="s">
+      <c r="AB3" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="AC3" s="6" t="s">
+      <c r="AC3" s="5" t="s">
         <v>14</v>
       </c>
-      <c r="AD3" s="24" t="s">
+      <c r="AD3" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="AE3" s="9"/>
-      <c r="AF3" s="5"/>
-      <c r="AG3" s="6" t="s">
+      <c r="AE3" s="8"/>
+      <c r="AF3" s="4"/>
+      <c r="AG3" s="5" t="s">
         <v>27</v>
       </c>
-      <c r="AH3" s="6" t="s">
+      <c r="AH3" s="5" t="s">
         <v>71</v>
       </c>
-      <c r="AI3" s="6" t="s">
+      <c r="AI3" s="5" t="s">
         <v>17</v>
       </c>
-      <c r="AJ3" s="8" t="s">
+      <c r="AJ3" s="7" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="10" t="s">
+      <c r="B4" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="C4" s="11" t="s">
+      <c r="C4" s="10" t="s">
         <v>35</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="11" t="s">
         <v>43</v>
       </c>
-      <c r="E4" s="11" t="s">
+      <c r="E4" s="10" t="s">
         <v>36</v>
       </c>
-      <c r="F4" s="13" t="s">
+      <c r="F4" s="12" t="s">
         <v>46</v>
       </c>
-      <c r="G4" s="9"/>
-      <c r="H4" s="10" t="s">
+      <c r="G4" s="8"/>
+      <c r="H4" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="I4" s="11" t="s">
+      <c r="I4" s="10" t="s">
         <v>56</v>
       </c>
-      <c r="J4" s="11" t="s">
+      <c r="J4" s="10" t="s">
         <v>34</v>
       </c>
-      <c r="K4" s="11" t="s">
+      <c r="K4" s="10" t="s">
         <v>39</v>
       </c>
-      <c r="L4" s="13" t="s">
+      <c r="L4" s="12" t="s">
         <v>40</v>
       </c>
-      <c r="N4" s="10" t="s">
+      <c r="N4" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="O4" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="O4" s="11" t="s">
+      <c r="P4" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="Q4" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="P4" s="43" t="s">
-        <v>95</v>
-      </c>
-      <c r="Q4" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="R4" s="13"/>
-      <c r="S4" s="9"/>
-      <c r="T4" s="29" t="s">
+      <c r="R4" s="12"/>
+      <c r="S4" s="8"/>
+      <c r="T4" s="28" t="s">
         <v>73</v>
       </c>
-      <c r="U4" s="28" t="s">
+      <c r="U4" s="27" t="s">
         <v>9</v>
       </c>
-      <c r="V4" s="28" t="s">
+      <c r="V4" s="27" t="s">
         <v>8</v>
       </c>
-      <c r="W4" s="28" t="s">
+      <c r="W4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="X4" s="30" t="s">
+      <c r="X4" s="29" t="s">
         <v>74</v>
       </c>
-      <c r="Z4" s="10" t="s">
+      <c r="Z4" s="9" t="s">
         <v>21</v>
       </c>
-      <c r="AA4" s="11" t="s">
+      <c r="AA4" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="AB4" s="12" t="s">
+      <c r="AB4" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="AC4" s="11" t="s">
+      <c r="AC4" s="10" t="s">
         <v>18</v>
       </c>
-      <c r="AD4" s="27" t="s">
+      <c r="AD4" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="AE4" s="9"/>
-      <c r="AF4" s="10" t="s">
+      <c r="AE4" s="8"/>
+      <c r="AF4" s="9" t="s">
         <v>31</v>
       </c>
-      <c r="AG4" s="36" t="s">
+      <c r="AG4" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="AH4" s="11" t="s">
+      <c r="AH4" s="10" t="s">
         <v>26</v>
       </c>
-      <c r="AI4" s="11" t="s">
+      <c r="AI4" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="AJ4" s="13" t="s">
+      <c r="AJ4" s="12" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="5" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="C5" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="D5" s="16" t="s">
+      <c r="D5" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="E5" s="11" t="s">
+      <c r="E5" s="10" t="s">
         <v>44</v>
       </c>
-      <c r="F5" s="12" t="s">
+      <c r="F5" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="G5" s="17"/>
-      <c r="H5" s="10" t="s">
+      <c r="G5" s="16"/>
+      <c r="H5" s="9" t="s">
         <v>49</v>
       </c>
-      <c r="I5" s="11" t="s">
+      <c r="I5" s="10" t="s">
         <v>47</v>
       </c>
-      <c r="J5" s="15" t="s">
+      <c r="J5" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="K5" s="15" t="s">
+      <c r="K5" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="L5" s="18" t="s">
+      <c r="L5" s="17" t="s">
         <v>2</v>
       </c>
-      <c r="N5" s="14"/>
-      <c r="O5" s="15"/>
-      <c r="P5" s="16"/>
-      <c r="Q5" s="11"/>
-      <c r="R5" s="12"/>
-      <c r="S5" s="17"/>
-      <c r="T5" s="10" t="s">
+      <c r="N5" s="13"/>
+      <c r="O5" s="14"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="10"/>
+      <c r="R5" s="11"/>
+      <c r="S5" s="16"/>
+      <c r="T5" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="U5" s="32" t="s">
+      <c r="U5" s="31" t="s">
         <v>79</v>
       </c>
-      <c r="V5" s="33" t="s">
+      <c r="V5" s="32" t="s">
         <v>77</v>
       </c>
-      <c r="W5" s="33" t="s">
+      <c r="W5" s="32" t="s">
         <v>16</v>
       </c>
-      <c r="X5" s="18"/>
-      <c r="Z5" s="14" t="s">
+      <c r="X5" s="17"/>
+      <c r="Z5" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="AA5" s="15" t="s">
+      <c r="AA5" s="14" t="s">
         <v>25</v>
       </c>
-      <c r="AB5" s="38" t="s">
+      <c r="AB5" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="AC5" s="11" t="s">
+      <c r="AC5" s="10" t="s">
         <v>23</v>
       </c>
-      <c r="AD5" s="31" t="s">
+      <c r="AD5" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="AE5" s="17"/>
-      <c r="AF5" s="10"/>
-      <c r="AG5" s="11" t="s">
+      <c r="AE5" s="16"/>
+      <c r="AF5" s="9"/>
+      <c r="AG5" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="AH5" s="15" t="s">
+      <c r="AH5" s="14" t="s">
         <v>70</v>
       </c>
-      <c r="AI5" s="15" t="s">
+      <c r="AI5" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="AJ5" s="18" t="s">
+      <c r="AJ5" s="17" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="6" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B6" s="9"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="47" t="s">
-        <v>100</v>
-      </c>
-      <c r="F6" s="46" t="s">
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="18"/>
+      <c r="E6" s="46" t="s">
         <v>99</v>
       </c>
-      <c r="G6" s="17"/>
-      <c r="H6" s="21" t="s">
+      <c r="F6" s="45" t="s">
+        <v>98</v>
+      </c>
+      <c r="G6" s="16"/>
+      <c r="H6" s="20" t="s">
         <v>76</v>
       </c>
-      <c r="I6" s="47" t="s">
+      <c r="I6" s="46" t="s">
         <v>77</v>
       </c>
-      <c r="J6" s="9"/>
-      <c r="K6" s="9"/>
-      <c r="L6" s="9"/>
-      <c r="N6" s="9"/>
-      <c r="O6" s="9"/>
-      <c r="P6" s="19"/>
-      <c r="Q6" s="14"/>
-      <c r="R6" s="20"/>
-      <c r="S6" s="17"/>
-      <c r="T6" s="4"/>
-      <c r="U6" s="22"/>
-      <c r="V6" s="9"/>
-      <c r="W6" s="9"/>
-      <c r="X6" s="9"/>
-      <c r="Z6" s="9"/>
-      <c r="AA6" s="9"/>
-      <c r="AB6" s="19"/>
-      <c r="AC6" s="2"/>
-      <c r="AD6" s="20"/>
-      <c r="AE6" s="17"/>
-      <c r="AF6" s="21"/>
-      <c r="AG6" s="20"/>
-      <c r="AH6" s="9"/>
-      <c r="AI6" s="9"/>
-      <c r="AJ6" s="9"/>
+      <c r="J6" s="8"/>
+      <c r="K6" s="8"/>
+      <c r="L6" s="8"/>
+      <c r="N6" s="8"/>
+      <c r="O6" s="8"/>
+      <c r="P6" s="18"/>
+      <c r="Q6" s="13"/>
+      <c r="R6" s="19"/>
+      <c r="S6" s="16"/>
+      <c r="T6" s="3"/>
+      <c r="U6" s="21"/>
+      <c r="V6" s="8"/>
+      <c r="W6" s="8"/>
+      <c r="X6" s="8"/>
+      <c r="Z6" s="8"/>
+      <c r="AA6" s="8"/>
+      <c r="AB6" s="18"/>
+      <c r="AC6" s="50"/>
+      <c r="AD6" s="19"/>
+      <c r="AE6" s="16"/>
+      <c r="AF6" s="20"/>
+      <c r="AG6" s="41"/>
+      <c r="AH6" s="8"/>
+      <c r="AI6" s="8"/>
+      <c r="AJ6" s="8"/>
     </row>
     <row r="7" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="E7" s="23"/>
+      <c r="E7" s="22"/>
     </row>
     <row r="8" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="50" t="s">
-        <v>85</v>
-      </c>
-      <c r="C8" s="50"/>
-      <c r="D8" s="50"/>
-      <c r="E8" s="50"/>
-      <c r="F8" s="50"/>
-      <c r="G8" s="50"/>
-      <c r="H8" s="50"/>
-      <c r="I8" s="50"/>
-      <c r="J8" s="50"/>
-      <c r="K8" s="50"/>
-      <c r="L8" s="50"/>
-      <c r="N8" s="50" t="s">
+      <c r="B8" s="49" t="s">
+        <v>101</v>
+      </c>
+      <c r="C8" s="49"/>
+      <c r="D8" s="49"/>
+      <c r="E8" s="49"/>
+      <c r="F8" s="49"/>
+      <c r="G8" s="49"/>
+      <c r="H8" s="49"/>
+      <c r="I8" s="49"/>
+      <c r="J8" s="49"/>
+      <c r="K8" s="49"/>
+      <c r="L8" s="49"/>
+      <c r="N8" s="49" t="s">
         <v>84</v>
       </c>
-      <c r="O8" s="50"/>
-      <c r="P8" s="50"/>
-      <c r="Q8" s="50"/>
-      <c r="R8" s="50"/>
-      <c r="S8" s="50"/>
-      <c r="T8" s="50"/>
-      <c r="U8" s="50"/>
-      <c r="V8" s="50"/>
-      <c r="W8" s="50"/>
-      <c r="X8" s="50"/>
-      <c r="Z8" s="51"/>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
-      <c r="AC8" s="51"/>
-      <c r="AD8" s="51"/>
-      <c r="AE8" s="51"/>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
+      <c r="O8" s="49"/>
+      <c r="P8" s="49"/>
+      <c r="Q8" s="49"/>
+      <c r="R8" s="49"/>
+      <c r="S8" s="49"/>
+      <c r="T8" s="49"/>
+      <c r="U8" s="49"/>
+      <c r="V8" s="49"/>
+      <c r="W8" s="49"/>
+      <c r="X8" s="49"/>
+      <c r="Z8" s="49" t="s">
+        <v>102</v>
+      </c>
+      <c r="AA8" s="49"/>
+      <c r="AB8" s="49"/>
+      <c r="AC8" s="49"/>
+      <c r="AD8" s="49"/>
+      <c r="AE8" s="49"/>
+      <c r="AF8" s="49"/>
+      <c r="AG8" s="49"/>
+      <c r="AH8" s="49"/>
+      <c r="AI8" s="49"/>
+      <c r="AJ8" s="49"/>
     </row>
     <row r="9" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="49" t="s">
+      <c r="B9" s="48" t="s">
+        <v>88</v>
+      </c>
+      <c r="C9" s="5"/>
+      <c r="D9" s="6"/>
+      <c r="E9" s="5"/>
+      <c r="F9" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="G9" s="8"/>
+      <c r="H9" s="4" t="s">
         <v>89</v>
       </c>
-      <c r="C9" s="6"/>
-      <c r="D9" s="7"/>
-      <c r="E9" s="6"/>
-      <c r="F9" s="8" t="s">
-        <v>86</v>
-      </c>
-      <c r="G9" s="9"/>
-      <c r="H9" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="I9" s="6"/>
-      <c r="J9" s="6"/>
-      <c r="K9" s="6"/>
-      <c r="L9" s="48" t="s">
-        <v>89</v>
-      </c>
-      <c r="N9" s="34" t="s">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5"/>
+      <c r="K9" s="5"/>
+      <c r="L9" s="47" t="s">
+        <v>88</v>
+      </c>
+      <c r="N9" s="33" t="s">
         <v>25</v>
       </c>
-      <c r="O9" s="39" t="s">
+      <c r="O9" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="P9" s="35" t="s">
+      <c r="P9" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="Q9" s="39" t="s">
+      <c r="Q9" s="38" t="s">
         <v>14</v>
       </c>
-      <c r="R9" s="24" t="s">
+      <c r="R9" s="23" t="s">
         <v>4</v>
       </c>
-      <c r="S9" s="9"/>
-      <c r="T9" s="5"/>
-      <c r="U9" s="6" t="s">
+      <c r="S9" s="8"/>
+      <c r="T9" s="4"/>
+      <c r="U9" s="5"/>
+      <c r="V9" s="5"/>
+      <c r="W9" s="5"/>
+      <c r="X9" s="7"/>
+      <c r="Z9" s="33"/>
+      <c r="AA9" s="38"/>
+      <c r="AB9" s="34"/>
+      <c r="AC9" s="38"/>
+      <c r="AD9" s="23"/>
+      <c r="AE9" s="8"/>
+      <c r="AF9" s="4"/>
+      <c r="AG9" s="5" t="s">
         <v>68</v>
       </c>
-      <c r="V9" s="6" t="s">
+      <c r="AH9" s="5" t="s">
         <v>69</v>
       </c>
-      <c r="W9" s="6"/>
-      <c r="X9" s="8"/>
-      <c r="Z9"/>
-      <c r="AA9"/>
-      <c r="AB9"/>
-      <c r="AC9"/>
-      <c r="AD9"/>
-      <c r="AE9"/>
-      <c r="AF9" s="40"/>
-      <c r="AG9"/>
-      <c r="AH9"/>
-      <c r="AI9"/>
-      <c r="AJ9"/>
+      <c r="AI9" s="5"/>
+      <c r="AJ9" s="7"/>
     </row>
     <row r="10" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="10" t="s">
+      <c r="B10" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="C10" s="10" t="s">
         <v>96</v>
       </c>
-      <c r="C10" s="11" t="s">
+      <c r="D10" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="E10" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="D10" s="43" t="s">
+      <c r="F10" s="12" t="s">
+        <v>86</v>
+      </c>
+      <c r="G10" s="8"/>
+      <c r="H10" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="I10" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="J10" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="L10" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="E10" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="F10" s="13" t="s">
-        <v>87</v>
-      </c>
-      <c r="G10" s="9"/>
-      <c r="H10" s="10" t="s">
-        <v>91</v>
-      </c>
-      <c r="I10" s="11" t="s">
-        <v>98</v>
-      </c>
-      <c r="J10" s="11" t="s">
+      <c r="N10" s="9">
+        <v>4</v>
+      </c>
+      <c r="O10" s="10">
+        <v>3</v>
+      </c>
+      <c r="P10" s="11">
+        <v>2</v>
+      </c>
+      <c r="Q10" s="10">
+        <v>1</v>
+      </c>
+      <c r="R10" s="26">
+        <v>0</v>
+      </c>
+      <c r="S10" s="8"/>
+      <c r="T10" s="9"/>
+      <c r="U10" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="V10" s="10" t="s">
+        <v>94</v>
+      </c>
+      <c r="W10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="X10" s="12" t="s">
         <v>95</v>
       </c>
-      <c r="K10" s="11" t="s">
+      <c r="Z10" s="9" t="s">
+        <v>95</v>
+      </c>
+      <c r="AA10" s="10" t="s">
+        <v>96</v>
+      </c>
+      <c r="AB10" s="42" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC10" s="10" t="s">
         <v>97</v>
       </c>
-      <c r="L10" s="13" t="s">
-        <v>96</v>
-      </c>
-      <c r="N10" s="10">
-        <v>4</v>
-      </c>
-      <c r="O10" s="11">
-        <v>3</v>
-      </c>
-      <c r="P10" s="12">
-        <v>2</v>
-      </c>
-      <c r="Q10" s="11">
-        <v>1</v>
-      </c>
-      <c r="R10" s="27">
-        <v>0</v>
-      </c>
-      <c r="S10" s="9"/>
-      <c r="T10" s="10" t="s">
+      <c r="AD10" s="26"/>
+      <c r="AE10" s="8"/>
+      <c r="AF10" s="9" t="s">
         <v>67</v>
       </c>
-      <c r="U10" s="11" t="s">
+      <c r="AG10" s="10" t="s">
         <v>58</v>
       </c>
-      <c r="V10" s="11" t="s">
+      <c r="AH10" s="10" t="s">
         <v>59</v>
       </c>
-      <c r="W10" s="11" t="s">
+      <c r="AI10" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="X10" s="13" t="s">
+      <c r="AJ10" s="12" t="s">
         <v>61</v>
       </c>
-      <c r="Z10"/>
-      <c r="AA10"/>
-      <c r="AB10"/>
-      <c r="AC10"/>
-      <c r="AD10"/>
-      <c r="AE10"/>
-      <c r="AF10" s="40"/>
-      <c r="AG10"/>
-      <c r="AH10"/>
-      <c r="AI10"/>
-      <c r="AJ10"/>
     </row>
     <row r="11" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="36" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" s="14"/>
+      <c r="D11" s="15"/>
+      <c r="E11" s="10"/>
+      <c r="F11" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="G11" s="16"/>
+      <c r="H11" s="9" t="s">
+        <v>91</v>
+      </c>
+      <c r="I11" s="10"/>
+      <c r="J11" s="10"/>
+      <c r="K11" s="10" t="s">
         <v>93</v>
       </c>
-      <c r="C11" s="15"/>
-      <c r="D11" s="16"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="12" t="s">
-        <v>88</v>
-      </c>
-      <c r="G11" s="17"/>
-      <c r="H11" s="10" t="s">
+      <c r="L11" s="12" t="s">
         <v>92</v>
       </c>
-      <c r="I11" s="11"/>
-      <c r="J11" s="11"/>
-      <c r="K11" s="11" t="s">
-        <v>94</v>
-      </c>
-      <c r="L11" s="13" t="s">
-        <v>93</v>
-      </c>
-      <c r="N11" s="14">
+      <c r="N11" s="13">
         <v>9</v>
       </c>
-      <c r="O11" s="15">
+      <c r="O11" s="14">
         <v>8</v>
       </c>
-      <c r="P11" s="16">
+      <c r="P11" s="15">
         <v>7</v>
       </c>
-      <c r="Q11" s="11">
+      <c r="Q11" s="10">
         <v>6</v>
       </c>
-      <c r="R11" s="31">
+      <c r="R11" s="30">
         <v>5</v>
       </c>
-      <c r="S11" s="17"/>
-      <c r="T11" s="10" t="s">
+      <c r="S11" s="16"/>
+      <c r="T11" s="9"/>
+      <c r="U11" s="10"/>
+      <c r="V11" s="14"/>
+      <c r="W11" s="14"/>
+      <c r="X11" s="17"/>
+      <c r="Z11" s="13" t="s">
+        <v>104</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="AB11" s="15" t="s">
+        <v>105</v>
+      </c>
+      <c r="AC11" s="10"/>
+      <c r="AD11" s="30" t="s">
+        <v>106</v>
+      </c>
+      <c r="AE11" s="16"/>
+      <c r="AF11" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="U11" s="11" t="s">
+      <c r="AG11" s="10" t="s">
         <v>63</v>
       </c>
-      <c r="V11" s="15" t="s">
+      <c r="AH11" s="14" t="s">
         <v>64</v>
       </c>
-      <c r="W11" s="15" t="s">
+      <c r="AI11" s="14" t="s">
         <v>65</v>
       </c>
-      <c r="X11" s="18" t="s">
+      <c r="AJ11" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="Z11" s="40"/>
-      <c r="AA11"/>
-      <c r="AB11"/>
-      <c r="AC11"/>
-      <c r="AD11"/>
-      <c r="AE11"/>
-      <c r="AF11" s="40"/>
-      <c r="AG11"/>
-      <c r="AH11"/>
-      <c r="AI11"/>
-      <c r="AJ11" s="40"/>
     </row>
     <row r="12" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B12" s="9"/>
-      <c r="C12" s="9"/>
-      <c r="D12" s="19"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="42"/>
-      <c r="G12" s="17"/>
-      <c r="H12" s="44"/>
-      <c r="I12" s="45"/>
-      <c r="J12" s="9"/>
-      <c r="K12" s="9"/>
-      <c r="L12" s="9"/>
-      <c r="N12" s="9"/>
-      <c r="O12" s="9"/>
-      <c r="P12" s="19"/>
-      <c r="Q12" s="14"/>
-      <c r="R12" s="3"/>
-      <c r="S12" s="17"/>
-      <c r="T12" s="21"/>
-      <c r="U12" s="22"/>
-      <c r="V12" s="9"/>
-      <c r="W12" s="9"/>
-      <c r="X12" s="9"/>
-      <c r="Z12"/>
-      <c r="AA12"/>
-      <c r="AB12"/>
-      <c r="AC12"/>
-      <c r="AD12"/>
-      <c r="AE12"/>
-      <c r="AF12"/>
-      <c r="AG12"/>
-      <c r="AH12"/>
-      <c r="AI12"/>
-      <c r="AJ12"/>
+      <c r="B12" s="8"/>
+      <c r="C12" s="8"/>
+      <c r="D12" s="18"/>
+      <c r="E12" s="40"/>
+      <c r="F12" s="41"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="43"/>
+      <c r="I12" s="44"/>
+      <c r="J12" s="8"/>
+      <c r="K12" s="8"/>
+      <c r="L12" s="8"/>
+      <c r="N12" s="8"/>
+      <c r="O12" s="8"/>
+      <c r="P12" s="18"/>
+      <c r="Q12" s="13"/>
+      <c r="R12" s="2"/>
+      <c r="S12" s="16"/>
+      <c r="T12" s="20"/>
+      <c r="U12" s="21"/>
+      <c r="V12" s="8"/>
+      <c r="W12" s="8"/>
+      <c r="X12" s="8"/>
+      <c r="Z12" s="8"/>
+      <c r="AA12" s="8"/>
+      <c r="AB12" s="18"/>
+      <c r="AC12" s="40"/>
+      <c r="AD12" s="51"/>
+      <c r="AE12" s="16"/>
+      <c r="AF12" s="20"/>
+      <c r="AG12" s="21"/>
+      <c r="AH12" s="8"/>
+      <c r="AI12" s="8"/>
+      <c r="AJ12" s="8"/>
     </row>
     <row r="14" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="Z14"/>
       <c r="AA14"/>
-      <c r="AB14" s="40"/>
+      <c r="AB14" s="39"/>
       <c r="AC14"/>
-      <c r="AD14" s="40"/>
+      <c r="AD14" s="39"/>
       <c r="AK14"/>
       <c r="AL14"/>
       <c r="AM14"/>
@@ -1825,12 +1907,28 @@
       <c r="AO14"/>
       <c r="AP14"/>
     </row>
-    <row r="15" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B15" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="N15" s="49" t="s">
+        <v>81</v>
+      </c>
+      <c r="O15" s="49"/>
+      <c r="P15" s="49"/>
+      <c r="Q15" s="49"/>
+      <c r="R15" s="49"/>
+      <c r="S15" s="49"/>
+      <c r="T15" s="49"/>
+      <c r="U15" s="49"/>
+      <c r="V15" s="49"/>
+      <c r="W15" s="49"/>
+      <c r="X15" s="49"/>
       <c r="Z15"/>
       <c r="AA15"/>
       <c r="AB15"/>
       <c r="AC15"/>
-      <c r="AD15" s="40"/>
+      <c r="AD15" s="39"/>
       <c r="AK15"/>
       <c r="AL15"/>
       <c r="AM15"/>
@@ -1839,11 +1937,51 @@
       <c r="AP15"/>
     </row>
     <row r="16" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="1" t="s">
+        <v>108</v>
+      </c>
+      <c r="C16" s="1" t="s">
+        <v>109</v>
+      </c>
+      <c r="D16" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="N16" s="4">
+        <v>0</v>
+      </c>
+      <c r="O16" s="5">
+        <v>1</v>
+      </c>
+      <c r="P16" s="6">
+        <v>2</v>
+      </c>
+      <c r="Q16" s="5">
+        <v>3</v>
+      </c>
+      <c r="R16" s="7">
+        <v>4</v>
+      </c>
+      <c r="S16" s="8"/>
+      <c r="T16" s="4">
+        <v>5</v>
+      </c>
+      <c r="U16" s="5">
+        <v>6</v>
+      </c>
+      <c r="V16" s="5">
+        <v>7</v>
+      </c>
+      <c r="W16" s="5">
+        <v>8</v>
+      </c>
+      <c r="X16" s="7">
+        <v>9</v>
+      </c>
       <c r="Z16"/>
       <c r="AA16"/>
-      <c r="AB16" s="40"/>
+      <c r="AB16" s="39"/>
       <c r="AC16"/>
-      <c r="AD16" s="40"/>
+      <c r="AD16" s="39"/>
       <c r="AK16"/>
       <c r="AL16"/>
       <c r="AM16"/>
@@ -1851,7 +1989,47 @@
       <c r="AO16"/>
       <c r="AP16"/>
     </row>
-    <row r="17" spans="37:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>111</v>
+      </c>
+      <c r="D17" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="N17" s="9">
+        <v>10</v>
+      </c>
+      <c r="O17" s="10">
+        <v>11</v>
+      </c>
+      <c r="P17" s="11">
+        <v>12</v>
+      </c>
+      <c r="Q17" s="10">
+        <v>13</v>
+      </c>
+      <c r="R17" s="12">
+        <v>14</v>
+      </c>
+      <c r="S17" s="8"/>
+      <c r="T17" s="9">
+        <v>15</v>
+      </c>
+      <c r="U17" s="10">
+        <v>16</v>
+      </c>
+      <c r="V17" s="10">
+        <v>17</v>
+      </c>
+      <c r="W17" s="10">
+        <v>18</v>
+      </c>
+      <c r="X17" s="12">
+        <v>19</v>
+      </c>
       <c r="AK17"/>
       <c r="AL17"/>
       <c r="AM17"/>
@@ -1859,7 +2037,47 @@
       <c r="AO17"/>
       <c r="AP17"/>
     </row>
-    <row r="18" spans="37:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B18" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>112</v>
+      </c>
+      <c r="D18" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="N18" s="13">
+        <v>21</v>
+      </c>
+      <c r="O18" s="14">
+        <v>22</v>
+      </c>
+      <c r="P18" s="15">
+        <v>23</v>
+      </c>
+      <c r="Q18" s="10">
+        <v>24</v>
+      </c>
+      <c r="R18" s="11">
+        <v>25</v>
+      </c>
+      <c r="S18" s="16"/>
+      <c r="T18" s="9">
+        <v>26</v>
+      </c>
+      <c r="U18" s="10">
+        <v>27</v>
+      </c>
+      <c r="V18" s="14">
+        <v>28</v>
+      </c>
+      <c r="W18" s="14">
+        <v>29</v>
+      </c>
+      <c r="X18" s="17">
+        <v>30</v>
+      </c>
       <c r="AK18"/>
       <c r="AL18"/>
       <c r="AM18"/>
@@ -1867,8 +2085,47 @@
       <c r="AO18"/>
       <c r="AP18"/>
     </row>
+    <row r="19" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B19" s="1" t="s">
+        <v>113</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>114</v>
+      </c>
+      <c r="D19" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="N19" s="8"/>
+      <c r="O19" s="8"/>
+      <c r="P19" s="18"/>
+      <c r="Q19" s="46">
+        <v>31</v>
+      </c>
+      <c r="R19" s="45">
+        <v>32</v>
+      </c>
+      <c r="S19" s="16"/>
+      <c r="T19" s="20">
+        <v>33</v>
+      </c>
+      <c r="U19" s="46">
+        <v>34</v>
+      </c>
+      <c r="V19" s="8"/>
+      <c r="W19" s="8"/>
+      <c r="X19" s="8"/>
+    </row>
+    <row r="20" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="1" t="s">
+        <v>116</v>
+      </c>
+      <c r="D20" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="7">
+    <mergeCell ref="N15:X15"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="N8:X8"/>

</xml_diff>

<commit_message>
Going back to 3 key combos. Also implemented a .gitignore
</commit_message>
<xml_diff>
--- a/Urchin Layouts.xlsx
+++ b/Urchin Layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhsch\Documents\Development\zmk-urchin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F4D1C401-1B70-4890-AAC9-B9DFC8F481DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21612733-BDC4-4976-AEF7-CE7CB04D1DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-105" yWindow="0" windowWidth="9975" windowHeight="15585" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="9" r:id="rId1"/>
@@ -339,9 +339,6 @@
     <t>tab</t>
   </si>
   <si>
-    <t>A+R</t>
-  </si>
-  <si>
     <t>6 Settings</t>
   </si>
   <si>
@@ -363,21 +360,6 @@
     <t>Combos</t>
   </si>
   <si>
-    <t>S+T</t>
-  </si>
-  <si>
-    <t>N+E</t>
-  </si>
-  <si>
-    <t>R+S</t>
-  </si>
-  <si>
-    <t>E+I</t>
-  </si>
-  <si>
-    <t>I+O</t>
-  </si>
-  <si>
     <t>A+R+S+T</t>
   </si>
   <si>
@@ -388,6 +370,24 @@
   </si>
   <si>
     <t>S+E</t>
+  </si>
+  <si>
+    <t>A+R+S</t>
+  </si>
+  <si>
+    <t>R+S+T</t>
+  </si>
+  <si>
+    <t>A+R+T</t>
+  </si>
+  <si>
+    <t>N+E+I</t>
+  </si>
+  <si>
+    <t>E+I+O</t>
+  </si>
+  <si>
+    <t>N+I+O</t>
   </si>
 </sst>
 </file>
@@ -890,13 +890,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="9" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1244,8 +1244,8 @@
   </sheetPr>
   <dimension ref="B2:AP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="S1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R19" sqref="R19"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B20" sqref="B2:AJ20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1254,45 +1254,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="49" t="s">
+      <c r="B2" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="49"/>
-      <c r="D2" s="49"/>
-      <c r="E2" s="49"/>
-      <c r="F2" s="49"/>
-      <c r="G2" s="49"/>
-      <c r="H2" s="49"/>
-      <c r="I2" s="49"/>
-      <c r="J2" s="49"/>
-      <c r="K2" s="49"/>
-      <c r="L2" s="49"/>
-      <c r="N2" s="49" t="s">
+      <c r="C2" s="51"/>
+      <c r="D2" s="51"/>
+      <c r="E2" s="51"/>
+      <c r="F2" s="51"/>
+      <c r="G2" s="51"/>
+      <c r="H2" s="51"/>
+      <c r="I2" s="51"/>
+      <c r="J2" s="51"/>
+      <c r="K2" s="51"/>
+      <c r="L2" s="51"/>
+      <c r="N2" s="51" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="49"/>
-      <c r="P2" s="49"/>
-      <c r="Q2" s="49"/>
-      <c r="R2" s="49"/>
-      <c r="S2" s="49"/>
-      <c r="T2" s="49"/>
-      <c r="U2" s="49"/>
-      <c r="V2" s="49"/>
-      <c r="W2" s="49"/>
-      <c r="X2" s="49"/>
-      <c r="Z2" s="49" t="s">
+      <c r="O2" s="51"/>
+      <c r="P2" s="51"/>
+      <c r="Q2" s="51"/>
+      <c r="R2" s="51"/>
+      <c r="S2" s="51"/>
+      <c r="T2" s="51"/>
+      <c r="U2" s="51"/>
+      <c r="V2" s="51"/>
+      <c r="W2" s="51"/>
+      <c r="X2" s="51"/>
+      <c r="Z2" s="51" t="s">
         <v>83</v>
       </c>
-      <c r="AA2" s="49"/>
-      <c r="AB2" s="49"/>
-      <c r="AC2" s="49"/>
-      <c r="AD2" s="49"/>
-      <c r="AE2" s="49"/>
-      <c r="AF2" s="49"/>
-      <c r="AG2" s="49"/>
-      <c r="AH2" s="49"/>
-      <c r="AI2" s="49"/>
-      <c r="AJ2" s="49"/>
+      <c r="AA2" s="51"/>
+      <c r="AB2" s="51"/>
+      <c r="AC2" s="51"/>
+      <c r="AD2" s="51"/>
+      <c r="AE2" s="51"/>
+      <c r="AF2" s="51"/>
+      <c r="AG2" s="51"/>
+      <c r="AH2" s="51"/>
+      <c r="AI2" s="51"/>
+      <c r="AJ2" s="51"/>
     </row>
     <row r="3" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1585,7 +1585,7 @@
       <c r="Z6" s="8"/>
       <c r="AA6" s="8"/>
       <c r="AB6" s="18"/>
-      <c r="AC6" s="50"/>
+      <c r="AC6" s="49"/>
       <c r="AD6" s="19"/>
       <c r="AE6" s="16"/>
       <c r="AF6" s="20"/>
@@ -1598,45 +1598,45 @@
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="49" t="s">
+      <c r="B8" s="51" t="s">
+        <v>100</v>
+      </c>
+      <c r="C8" s="51"/>
+      <c r="D8" s="51"/>
+      <c r="E8" s="51"/>
+      <c r="F8" s="51"/>
+      <c r="G8" s="51"/>
+      <c r="H8" s="51"/>
+      <c r="I8" s="51"/>
+      <c r="J8" s="51"/>
+      <c r="K8" s="51"/>
+      <c r="L8" s="51"/>
+      <c r="N8" s="51" t="s">
+        <v>84</v>
+      </c>
+      <c r="O8" s="51"/>
+      <c r="P8" s="51"/>
+      <c r="Q8" s="51"/>
+      <c r="R8" s="51"/>
+      <c r="S8" s="51"/>
+      <c r="T8" s="51"/>
+      <c r="U8" s="51"/>
+      <c r="V8" s="51"/>
+      <c r="W8" s="51"/>
+      <c r="X8" s="51"/>
+      <c r="Z8" s="51" t="s">
         <v>101</v>
       </c>
-      <c r="C8" s="49"/>
-      <c r="D8" s="49"/>
-      <c r="E8" s="49"/>
-      <c r="F8" s="49"/>
-      <c r="G8" s="49"/>
-      <c r="H8" s="49"/>
-      <c r="I8" s="49"/>
-      <c r="J8" s="49"/>
-      <c r="K8" s="49"/>
-      <c r="L8" s="49"/>
-      <c r="N8" s="49" t="s">
-        <v>84</v>
-      </c>
-      <c r="O8" s="49"/>
-      <c r="P8" s="49"/>
-      <c r="Q8" s="49"/>
-      <c r="R8" s="49"/>
-      <c r="S8" s="49"/>
-      <c r="T8" s="49"/>
-      <c r="U8" s="49"/>
-      <c r="V8" s="49"/>
-      <c r="W8" s="49"/>
-      <c r="X8" s="49"/>
-      <c r="Z8" s="49" t="s">
-        <v>102</v>
-      </c>
-      <c r="AA8" s="49"/>
-      <c r="AB8" s="49"/>
-      <c r="AC8" s="49"/>
-      <c r="AD8" s="49"/>
-      <c r="AE8" s="49"/>
-      <c r="AF8" s="49"/>
-      <c r="AG8" s="49"/>
-      <c r="AH8" s="49"/>
-      <c r="AI8" s="49"/>
-      <c r="AJ8" s="49"/>
+      <c r="AA8" s="51"/>
+      <c r="AB8" s="51"/>
+      <c r="AC8" s="51"/>
+      <c r="AD8" s="51"/>
+      <c r="AE8" s="51"/>
+      <c r="AF8" s="51"/>
+      <c r="AG8" s="51"/>
+      <c r="AH8" s="51"/>
+      <c r="AI8" s="51"/>
+      <c r="AJ8" s="51"/>
     </row>
     <row r="9" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
@@ -1830,17 +1830,17 @@
       <c r="W11" s="14"/>
       <c r="X11" s="17"/>
       <c r="Z11" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="AA11" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="AB11" s="15" t="s">
         <v>104</v>
-      </c>
-      <c r="AA11" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="AB11" s="15" t="s">
-        <v>105</v>
       </c>
       <c r="AC11" s="10"/>
       <c r="AD11" s="30" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="AE11" s="16"/>
       <c r="AF11" s="9" t="s">
@@ -1886,7 +1886,7 @@
       <c r="AA12" s="8"/>
       <c r="AB12" s="18"/>
       <c r="AC12" s="40"/>
-      <c r="AD12" s="51"/>
+      <c r="AD12" s="50"/>
       <c r="AE12" s="16"/>
       <c r="AF12" s="20"/>
       <c r="AG12" s="21"/>
@@ -1909,21 +1909,21 @@
     </row>
     <row r="15" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B15" s="1" t="s">
-        <v>107</v>
-      </c>
-      <c r="N15" s="49" t="s">
+        <v>106</v>
+      </c>
+      <c r="N15" s="51" t="s">
         <v>81</v>
       </c>
-      <c r="O15" s="49"/>
-      <c r="P15" s="49"/>
-      <c r="Q15" s="49"/>
-      <c r="R15" s="49"/>
-      <c r="S15" s="49"/>
-      <c r="T15" s="49"/>
-      <c r="U15" s="49"/>
-      <c r="V15" s="49"/>
-      <c r="W15" s="49"/>
-      <c r="X15" s="49"/>
+      <c r="O15" s="51"/>
+      <c r="P15" s="51"/>
+      <c r="Q15" s="51"/>
+      <c r="R15" s="51"/>
+      <c r="S15" s="51"/>
+      <c r="T15" s="51"/>
+      <c r="U15" s="51"/>
+      <c r="V15" s="51"/>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
       <c r="Z15"/>
       <c r="AA15"/>
       <c r="AB15"/>
@@ -1938,10 +1938,10 @@
     </row>
     <row r="16" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="1" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="C16" s="1" t="s">
-        <v>109</v>
+        <v>115</v>
       </c>
       <c r="D16" s="1" t="s">
         <v>97</v>
@@ -1991,10 +1991,10 @@
     </row>
     <row r="17" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="1" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
       <c r="C17" s="1" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="D17" s="1" t="s">
         <v>94</v>
@@ -2039,10 +2039,10 @@
     </row>
     <row r="18" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B18" s="1" t="s">
-        <v>100</v>
+        <v>113</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>112</v>
+        <v>116</v>
       </c>
       <c r="D18" s="1" t="s">
         <v>96</v>
@@ -2087,10 +2087,10 @@
     </row>
     <row r="19" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B19" s="1" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D19" s="1" t="s">
         <v>95</v>
@@ -2117,21 +2117,21 @@
     </row>
     <row r="20" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="Z8:AJ8"/>
+    <mergeCell ref="Z2:AJ2"/>
     <mergeCell ref="N15:X15"/>
     <mergeCell ref="B2:L2"/>
     <mergeCell ref="B8:L8"/>
     <mergeCell ref="N8:X8"/>
     <mergeCell ref="N2:X2"/>
-    <mergeCell ref="Z8:AJ8"/>
-    <mergeCell ref="Z2:AJ2"/>
   </mergeCells>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="landscape" r:id="rId1"/>

</xml_diff>

<commit_message>
Trying a one hand focused layout, larger use of combos
</commit_message>
<xml_diff>
--- a/Urchin Layouts.xlsx
+++ b/Urchin Layouts.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhsch\Documents\Development\zmk-urchin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21612733-BDC4-4976-AEF7-CE7CB04D1DE9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{25FB7811-8AE9-4B93-8B95-7E24CDB727F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
+    <workbookView xWindow="28680" yWindow="1050" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="9" r:id="rId1"/>
+    <sheet name="Artsey Inspired" sheetId="10" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="195">
   <si>
     <t>esc</t>
   </si>
@@ -388,13 +389,247 @@
   </si>
   <si>
     <t>N+I+O</t>
+  </si>
+  <si>
+    <t>q</t>
+  </si>
+  <si>
+    <t>Ring</t>
+  </si>
+  <si>
+    <t>Mid</t>
+  </si>
+  <si>
+    <t>Pnk</t>
+  </si>
+  <si>
+    <t>Pnt</t>
+  </si>
+  <si>
+    <t>Thmb</t>
+  </si>
+  <si>
+    <t>a</t>
+  </si>
+  <si>
+    <t>b</t>
+  </si>
+  <si>
+    <t>c</t>
+  </si>
+  <si>
+    <t>d</t>
+  </si>
+  <si>
+    <t>e</t>
+  </si>
+  <si>
+    <t>f</t>
+  </si>
+  <si>
+    <t>g</t>
+  </si>
+  <si>
+    <t>h</t>
+  </si>
+  <si>
+    <t>i</t>
+  </si>
+  <si>
+    <t>j</t>
+  </si>
+  <si>
+    <t>k</t>
+  </si>
+  <si>
+    <t>l</t>
+  </si>
+  <si>
+    <t>m</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>o</t>
+  </si>
+  <si>
+    <t>p</t>
+  </si>
+  <si>
+    <t>r</t>
+  </si>
+  <si>
+    <t>s</t>
+  </si>
+  <si>
+    <t>t</t>
+  </si>
+  <si>
+    <t>u</t>
+  </si>
+  <si>
+    <t>v</t>
+  </si>
+  <si>
+    <t>w</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>z</t>
+  </si>
+  <si>
+    <t>shft</t>
+  </si>
+  <si>
+    <t>Nav</t>
+  </si>
+  <si>
+    <t>Up</t>
+  </si>
+  <si>
+    <t>Dn</t>
+  </si>
+  <si>
+    <t>Rt</t>
+  </si>
+  <si>
+    <t>Lf</t>
+  </si>
+  <si>
+    <t>PU</t>
+  </si>
+  <si>
+    <t>PD</t>
+  </si>
+  <si>
+    <t>End</t>
+  </si>
+  <si>
+    <t>Num</t>
+  </si>
+  <si>
+    <t>Function</t>
+  </si>
+  <si>
+    <t>Alphas</t>
+  </si>
+  <si>
+    <t>nums</t>
+  </si>
+  <si>
+    <t>punctuation</t>
+  </si>
+  <si>
+    <t>"</t>
+  </si>
+  <si>
+    <t>:</t>
+  </si>
+  <si>
+    <t>symbols</t>
+  </si>
+  <si>
+    <t>brackets</t>
+  </si>
+  <si>
+    <t>nav</t>
+  </si>
+  <si>
+    <t>up</t>
+  </si>
+  <si>
+    <t>dn</t>
+  </si>
+  <si>
+    <t>left</t>
+  </si>
+  <si>
+    <t>right</t>
+  </si>
+  <si>
+    <t>mods</t>
+  </si>
+  <si>
+    <t>Other</t>
+  </si>
+  <si>
+    <t>space</t>
+  </si>
+  <si>
+    <t>enter</t>
+  </si>
+  <si>
+    <t>bkspc</t>
+  </si>
+  <si>
+    <t>delete</t>
+  </si>
+  <si>
+    <t>insert</t>
+  </si>
+  <si>
+    <t>caps wd</t>
+  </si>
+  <si>
+    <t>caps lk</t>
+  </si>
+  <si>
+    <t>function</t>
+  </si>
+  <si>
+    <t>Default</t>
+  </si>
+  <si>
+    <t>HOLD Layer</t>
+  </si>
+  <si>
+    <t>ToggleLayer</t>
+  </si>
+  <si>
+    <t>Flip</t>
+  </si>
+  <si>
+    <t>escape</t>
+  </si>
+  <si>
+    <t>Symbol</t>
+  </si>
+  <si>
+    <t>&lt;</t>
+  </si>
+  <si>
+    <t>&gt;</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>ctl+w</t>
+  </si>
+  <si>
+    <t>hm</t>
+  </si>
+  <si>
+    <t>escpe</t>
+  </si>
+  <si>
+    <t>capsword</t>
+  </si>
+  <si>
+    <t>inst</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -416,8 +651,29 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C5700"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -448,8 +704,13 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="22">
+  <borders count="31">
     <border>
       <left/>
       <right/>
@@ -742,11 +1003,126 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="74">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -896,11 +1272,69 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="22" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="24" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="25" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="26" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="27" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="23" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="2" quotePrefix="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="3">
+    <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
+    <cellStyle name="Neutral" xfId="2" builtinId="28"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1244,8 +1678,8 @@
   </sheetPr>
   <dimension ref="B2:AP20"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B20" sqref="B2:AJ20"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:L6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="5.7109375" defaultRowHeight="30" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1254,45 +1688,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="51" t="s">
+      <c r="B2" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="51"/>
-      <c r="D2" s="51"/>
-      <c r="E2" s="51"/>
-      <c r="F2" s="51"/>
-      <c r="G2" s="51"/>
-      <c r="H2" s="51"/>
-      <c r="I2" s="51"/>
-      <c r="J2" s="51"/>
-      <c r="K2" s="51"/>
-      <c r="L2" s="51"/>
-      <c r="N2" s="51" t="s">
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
+      <c r="N2" s="53" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="51"/>
-      <c r="P2" s="51"/>
-      <c r="Q2" s="51"/>
-      <c r="R2" s="51"/>
-      <c r="S2" s="51"/>
-      <c r="T2" s="51"/>
-      <c r="U2" s="51"/>
-      <c r="V2" s="51"/>
-      <c r="W2" s="51"/>
-      <c r="X2" s="51"/>
-      <c r="Z2" s="51" t="s">
+      <c r="O2" s="53"/>
+      <c r="P2" s="53"/>
+      <c r="Q2" s="53"/>
+      <c r="R2" s="53"/>
+      <c r="S2" s="53"/>
+      <c r="T2" s="53"/>
+      <c r="U2" s="53"/>
+      <c r="V2" s="53"/>
+      <c r="W2" s="53"/>
+      <c r="X2" s="53"/>
+      <c r="Z2" s="53" t="s">
         <v>83</v>
       </c>
-      <c r="AA2" s="51"/>
-      <c r="AB2" s="51"/>
-      <c r="AC2" s="51"/>
-      <c r="AD2" s="51"/>
-      <c r="AE2" s="51"/>
-      <c r="AF2" s="51"/>
-      <c r="AG2" s="51"/>
-      <c r="AH2" s="51"/>
-      <c r="AI2" s="51"/>
-      <c r="AJ2" s="51"/>
+      <c r="AA2" s="53"/>
+      <c r="AB2" s="53"/>
+      <c r="AC2" s="53"/>
+      <c r="AD2" s="53"/>
+      <c r="AE2" s="53"/>
+      <c r="AF2" s="53"/>
+      <c r="AG2" s="53"/>
+      <c r="AH2" s="53"/>
+      <c r="AI2" s="53"/>
+      <c r="AJ2" s="53"/>
     </row>
     <row r="3" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -1598,45 +2032,45 @@
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="51" t="s">
+      <c r="B8" s="53" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="51"/>
-      <c r="D8" s="51"/>
-      <c r="E8" s="51"/>
-      <c r="F8" s="51"/>
-      <c r="G8" s="51"/>
-      <c r="H8" s="51"/>
-      <c r="I8" s="51"/>
-      <c r="J8" s="51"/>
-      <c r="K8" s="51"/>
-      <c r="L8" s="51"/>
-      <c r="N8" s="51" t="s">
+      <c r="C8" s="53"/>
+      <c r="D8" s="53"/>
+      <c r="E8" s="53"/>
+      <c r="F8" s="53"/>
+      <c r="G8" s="53"/>
+      <c r="H8" s="53"/>
+      <c r="I8" s="53"/>
+      <c r="J8" s="53"/>
+      <c r="K8" s="53"/>
+      <c r="L8" s="53"/>
+      <c r="N8" s="53" t="s">
         <v>84</v>
       </c>
-      <c r="O8" s="51"/>
-      <c r="P8" s="51"/>
-      <c r="Q8" s="51"/>
-      <c r="R8" s="51"/>
-      <c r="S8" s="51"/>
-      <c r="T8" s="51"/>
-      <c r="U8" s="51"/>
-      <c r="V8" s="51"/>
-      <c r="W8" s="51"/>
-      <c r="X8" s="51"/>
-      <c r="Z8" s="51" t="s">
+      <c r="O8" s="53"/>
+      <c r="P8" s="53"/>
+      <c r="Q8" s="53"/>
+      <c r="R8" s="53"/>
+      <c r="S8" s="53"/>
+      <c r="T8" s="53"/>
+      <c r="U8" s="53"/>
+      <c r="V8" s="53"/>
+      <c r="W8" s="53"/>
+      <c r="X8" s="53"/>
+      <c r="Z8" s="53" t="s">
         <v>101</v>
       </c>
-      <c r="AA8" s="51"/>
-      <c r="AB8" s="51"/>
-      <c r="AC8" s="51"/>
-      <c r="AD8" s="51"/>
-      <c r="AE8" s="51"/>
-      <c r="AF8" s="51"/>
-      <c r="AG8" s="51"/>
-      <c r="AH8" s="51"/>
-      <c r="AI8" s="51"/>
-      <c r="AJ8" s="51"/>
+      <c r="AA8" s="53"/>
+      <c r="AB8" s="53"/>
+      <c r="AC8" s="53"/>
+      <c r="AD8" s="53"/>
+      <c r="AE8" s="53"/>
+      <c r="AF8" s="53"/>
+      <c r="AG8" s="53"/>
+      <c r="AH8" s="53"/>
+      <c r="AI8" s="53"/>
+      <c r="AJ8" s="53"/>
     </row>
     <row r="9" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
@@ -1911,19 +2345,19 @@
       <c r="B15" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N15" s="51" t="s">
+      <c r="N15" s="53" t="s">
         <v>81</v>
       </c>
-      <c r="O15" s="51"/>
-      <c r="P15" s="51"/>
-      <c r="Q15" s="51"/>
-      <c r="R15" s="51"/>
-      <c r="S15" s="51"/>
-      <c r="T15" s="51"/>
-      <c r="U15" s="51"/>
-      <c r="V15" s="51"/>
-      <c r="W15" s="51"/>
-      <c r="X15" s="51"/>
+      <c r="O15" s="53"/>
+      <c r="P15" s="53"/>
+      <c r="Q15" s="53"/>
+      <c r="R15" s="53"/>
+      <c r="S15" s="53"/>
+      <c r="T15" s="53"/>
+      <c r="U15" s="53"/>
+      <c r="V15" s="53"/>
+      <c r="W15" s="53"/>
+      <c r="X15" s="53"/>
       <c r="Z15"/>
       <c r="AA15"/>
       <c r="AB15"/>
@@ -2136,4 +2570,1290 @@
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup scale="64" orientation="landscape" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92B8116D-64C5-4186-AF1F-3BF785B9A034}">
+  <dimension ref="A1:AD42"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="9.140625" style="51"/>
+    <col min="2" max="6" width="4.85546875" customWidth="1"/>
+    <col min="10" max="20" width="5.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C1" t="s">
+        <v>118</v>
+      </c>
+      <c r="D1" t="s">
+        <v>119</v>
+      </c>
+      <c r="E1" t="s">
+        <v>121</v>
+      </c>
+      <c r="F1" t="s">
+        <v>122</v>
+      </c>
+      <c r="I1" s="56"/>
+      <c r="J1" s="56"/>
+      <c r="K1" s="56"/>
+      <c r="L1" s="56"/>
+      <c r="M1" s="56"/>
+      <c r="N1" s="56"/>
+      <c r="O1" s="56"/>
+      <c r="P1" s="56"/>
+      <c r="Q1" s="56"/>
+      <c r="R1" s="56"/>
+      <c r="S1" s="56"/>
+      <c r="T1" s="56"/>
+      <c r="U1" s="56"/>
+    </row>
+    <row r="2" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A2" s="51" t="s">
+        <v>95</v>
+      </c>
+      <c r="B2">
+        <v>2</v>
+      </c>
+      <c r="C2">
+        <v>2</v>
+      </c>
+      <c r="D2">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>2</v>
+      </c>
+      <c r="I2" s="56"/>
+      <c r="J2" s="10">
+        <v>1</v>
+      </c>
+      <c r="K2" s="10">
+        <v>1</v>
+      </c>
+      <c r="L2" s="10">
+        <v>1</v>
+      </c>
+      <c r="M2" s="10">
+        <v>1</v>
+      </c>
+      <c r="N2" s="10">
+        <v>4</v>
+      </c>
+      <c r="O2" s="57"/>
+      <c r="P2" s="10">
+        <v>4</v>
+      </c>
+      <c r="Q2" s="10">
+        <v>1</v>
+      </c>
+      <c r="R2" s="10">
+        <v>1</v>
+      </c>
+      <c r="S2" s="10">
+        <v>1</v>
+      </c>
+      <c r="T2" s="10">
+        <v>1</v>
+      </c>
+      <c r="U2" s="56"/>
+    </row>
+    <row r="3" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A3" s="51" t="s">
+        <v>96</v>
+      </c>
+      <c r="B3">
+        <v>2</v>
+      </c>
+      <c r="C3">
+        <v>2</v>
+      </c>
+      <c r="E3">
+        <v>2</v>
+      </c>
+      <c r="I3" s="56"/>
+      <c r="J3" s="10">
+        <v>2</v>
+      </c>
+      <c r="K3" s="10">
+        <v>2</v>
+      </c>
+      <c r="L3" s="10">
+        <v>2</v>
+      </c>
+      <c r="M3" s="10">
+        <v>2</v>
+      </c>
+      <c r="N3" s="10">
+        <v>5</v>
+      </c>
+      <c r="O3" s="57"/>
+      <c r="P3" s="10">
+        <v>5</v>
+      </c>
+      <c r="Q3" s="10">
+        <v>2</v>
+      </c>
+      <c r="R3" s="10">
+        <v>2</v>
+      </c>
+      <c r="S3" s="10">
+        <v>2</v>
+      </c>
+      <c r="T3" s="10">
+        <v>2</v>
+      </c>
+      <c r="U3" s="56"/>
+      <c r="V3">
+        <f>COUNTA(V5:V32)</f>
+        <v>26</v>
+      </c>
+      <c r="W3">
+        <f t="shared" ref="W3:AA3" si="0">COUNTA(W5:W32)</f>
+        <v>10</v>
+      </c>
+      <c r="X3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+      <c r="Y3">
+        <f t="shared" si="0"/>
+        <v>14</v>
+      </c>
+      <c r="Z3">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="AA3">
+        <f t="shared" si="0"/>
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="51" t="s">
+        <v>94</v>
+      </c>
+      <c r="C4">
+        <v>2</v>
+      </c>
+      <c r="D4">
+        <v>2</v>
+      </c>
+      <c r="E4">
+        <v>2</v>
+      </c>
+      <c r="I4" s="56"/>
+      <c r="J4" s="10">
+        <v>3</v>
+      </c>
+      <c r="K4" s="10">
+        <v>3</v>
+      </c>
+      <c r="L4" s="10">
+        <v>3</v>
+      </c>
+      <c r="M4" s="10">
+        <v>3</v>
+      </c>
+      <c r="N4" s="10">
+        <v>6</v>
+      </c>
+      <c r="O4" s="57"/>
+      <c r="P4" s="10">
+        <v>6</v>
+      </c>
+      <c r="Q4" s="10">
+        <v>3</v>
+      </c>
+      <c r="R4" s="10">
+        <v>3</v>
+      </c>
+      <c r="S4" s="10">
+        <v>3</v>
+      </c>
+      <c r="T4" s="35">
+        <v>3</v>
+      </c>
+      <c r="U4" s="56"/>
+      <c r="V4" s="54" t="s">
+        <v>159</v>
+      </c>
+      <c r="W4" s="54" t="s">
+        <v>160</v>
+      </c>
+      <c r="X4" s="54" t="s">
+        <v>161</v>
+      </c>
+      <c r="Y4" s="54" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z4" s="54" t="s">
+        <v>165</v>
+      </c>
+      <c r="AA4" s="54" t="s">
+        <v>166</v>
+      </c>
+      <c r="AB4" s="54" t="s">
+        <v>171</v>
+      </c>
+      <c r="AC4" s="54" t="s">
+        <v>172</v>
+      </c>
+      <c r="AD4" s="55" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="5" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A5" s="51" t="s">
+        <v>97</v>
+      </c>
+      <c r="B5">
+        <v>2</v>
+      </c>
+      <c r="C5">
+        <v>2</v>
+      </c>
+      <c r="D5">
+        <v>2</v>
+      </c>
+      <c r="I5" s="56"/>
+      <c r="J5" s="57"/>
+      <c r="K5" s="57"/>
+      <c r="L5" s="57"/>
+      <c r="M5" s="58">
+        <v>2</v>
+      </c>
+      <c r="N5" s="58">
+        <v>1</v>
+      </c>
+      <c r="O5" s="57"/>
+      <c r="P5" s="10">
+        <v>1</v>
+      </c>
+      <c r="Q5" s="58">
+        <v>2</v>
+      </c>
+      <c r="R5" s="57"/>
+      <c r="S5" s="57"/>
+      <c r="T5" s="57"/>
+      <c r="U5" s="56"/>
+      <c r="V5" s="67" t="s">
+        <v>123</v>
+      </c>
+      <c r="W5" s="67">
+        <v>0</v>
+      </c>
+      <c r="X5" s="67" t="s">
+        <v>5</v>
+      </c>
+      <c r="Y5" s="67" t="s">
+        <v>10</v>
+      </c>
+      <c r="Z5" s="67" t="s">
+        <v>26</v>
+      </c>
+      <c r="AA5" s="67" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB5" s="67" t="s">
+        <v>97</v>
+      </c>
+      <c r="AC5" s="67" t="s">
+        <v>173</v>
+      </c>
+      <c r="AD5" s="67" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="6" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A6" s="51" t="s">
+        <v>192</v>
+      </c>
+      <c r="B6">
+        <v>1</v>
+      </c>
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="I6" s="56"/>
+      <c r="J6" s="56"/>
+      <c r="K6" s="56"/>
+      <c r="L6" s="56"/>
+      <c r="M6" s="56"/>
+      <c r="N6" s="56"/>
+      <c r="O6" s="56"/>
+      <c r="P6" s="56"/>
+      <c r="Q6" s="56"/>
+      <c r="R6" s="56"/>
+      <c r="S6" s="56"/>
+      <c r="T6" s="56"/>
+      <c r="U6" s="56"/>
+      <c r="V6" s="67" t="s">
+        <v>124</v>
+      </c>
+      <c r="W6" s="67">
+        <v>1</v>
+      </c>
+      <c r="X6" s="67" t="s">
+        <v>4</v>
+      </c>
+      <c r="Y6" s="67" t="s">
+        <v>17</v>
+      </c>
+      <c r="Z6" s="67" t="s">
+        <v>70</v>
+      </c>
+      <c r="AA6" s="67" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB6" s="67" t="s">
+        <v>96</v>
+      </c>
+      <c r="AC6" s="67" t="s">
+        <v>99</v>
+      </c>
+      <c r="AD6" s="67" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="7" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A7" s="51" t="s">
+        <v>193</v>
+      </c>
+      <c r="C7">
+        <v>2</v>
+      </c>
+      <c r="D7">
+        <v>2</v>
+      </c>
+      <c r="E7">
+        <v>5</v>
+      </c>
+      <c r="J7" t="s">
+        <v>181</v>
+      </c>
+      <c r="V7" s="67" t="s">
+        <v>125</v>
+      </c>
+      <c r="W7" s="67">
+        <v>2</v>
+      </c>
+      <c r="X7" s="67" t="s">
+        <v>71</v>
+      </c>
+      <c r="Y7" s="67" t="s">
+        <v>19</v>
+      </c>
+      <c r="Z7" s="67" t="s">
+        <v>13</v>
+      </c>
+      <c r="AA7" s="67" t="s">
+        <v>169</v>
+      </c>
+      <c r="AB7" s="67" t="s">
+        <v>94</v>
+      </c>
+      <c r="AC7" s="67" t="s">
+        <v>174</v>
+      </c>
+      <c r="AD7" s="67" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="8" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A8" s="51" t="s">
+        <v>99</v>
+      </c>
+      <c r="D8">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>1</v>
+      </c>
+      <c r="J8" s="10" t="s">
+        <v>117</v>
+      </c>
+      <c r="K8" s="10" t="s">
+        <v>144</v>
+      </c>
+      <c r="L8" s="10" t="s">
+        <v>128</v>
+      </c>
+      <c r="M8" s="10" t="s">
+        <v>138</v>
+      </c>
+      <c r="N8" s="10" t="s">
+        <v>124</v>
+      </c>
+      <c r="O8" s="57"/>
+      <c r="P8" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="Q8" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="R8" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="S8" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="T8" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="V8" s="67" t="s">
+        <v>126</v>
+      </c>
+      <c r="W8" s="67">
+        <v>3</v>
+      </c>
+      <c r="X8" s="67" t="s">
+        <v>18</v>
+      </c>
+      <c r="Y8" s="67" t="s">
+        <v>20</v>
+      </c>
+      <c r="Z8" s="67" t="s">
+        <v>12</v>
+      </c>
+      <c r="AA8" s="67" t="s">
+        <v>170</v>
+      </c>
+      <c r="AB8" s="67" t="s">
+        <v>95</v>
+      </c>
+      <c r="AC8" s="51" t="s">
+        <v>175</v>
+      </c>
+      <c r="AD8" s="67" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="9" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="J9" s="10" t="s">
+        <v>123</v>
+      </c>
+      <c r="K9" s="10" t="s">
+        <v>139</v>
+      </c>
+      <c r="L9" s="10" t="s">
+        <v>140</v>
+      </c>
+      <c r="M9" s="10" t="s">
+        <v>141</v>
+      </c>
+      <c r="N9" s="10" t="s">
+        <v>129</v>
+      </c>
+      <c r="O9" s="57"/>
+      <c r="P9" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="Q9" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="R9" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="S9" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="T9" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="V9" s="67" t="s">
+        <v>127</v>
+      </c>
+      <c r="W9" s="67">
+        <v>4</v>
+      </c>
+      <c r="X9" s="68" t="s">
+        <v>2</v>
+      </c>
+      <c r="Y9" s="67" t="s">
+        <v>21</v>
+      </c>
+      <c r="Z9" s="67" t="s">
+        <v>29</v>
+      </c>
+      <c r="AA9" s="67" t="s">
+        <v>78</v>
+      </c>
+      <c r="AB9" s="51"/>
+      <c r="AC9" s="51" t="s">
+        <v>176</v>
+      </c>
+      <c r="AD9" s="67" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="10" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="J10" s="10" t="s">
+        <v>147</v>
+      </c>
+      <c r="K10" s="10" t="s">
+        <v>145</v>
+      </c>
+      <c r="L10" s="10" t="s">
+        <v>125</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>126</v>
+      </c>
+      <c r="N10" s="10" t="s">
+        <v>143</v>
+      </c>
+      <c r="O10" s="57"/>
+      <c r="P10" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="Q10" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="R10" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="S10" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="T10" s="35" t="s">
+        <v>2</v>
+      </c>
+      <c r="V10" s="67" t="s">
+        <v>128</v>
+      </c>
+      <c r="W10" s="67">
+        <v>5</v>
+      </c>
+      <c r="X10" s="68" t="s">
+        <v>162</v>
+      </c>
+      <c r="Y10" s="67" t="s">
+        <v>22</v>
+      </c>
+      <c r="Z10" s="67" t="s">
+        <v>28</v>
+      </c>
+      <c r="AA10" s="67" t="s">
+        <v>79</v>
+      </c>
+      <c r="AB10" s="51"/>
+      <c r="AC10" s="51" t="s">
+        <v>177</v>
+      </c>
+      <c r="AD10" s="67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="11" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="J11" s="57"/>
+      <c r="K11" s="57"/>
+      <c r="L11" s="57"/>
+      <c r="M11" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="N11" s="58" t="s">
+        <v>98</v>
+      </c>
+      <c r="O11" s="57"/>
+      <c r="P11" s="10"/>
+      <c r="Q11" s="58"/>
+      <c r="R11" s="57"/>
+      <c r="S11" s="57"/>
+      <c r="T11" s="57"/>
+      <c r="V11" s="67" t="s">
+        <v>129</v>
+      </c>
+      <c r="W11" s="67">
+        <v>6</v>
+      </c>
+      <c r="X11" s="67" t="s">
+        <v>1</v>
+      </c>
+      <c r="Y11" s="67" t="s">
+        <v>23</v>
+      </c>
+      <c r="Z11" s="67" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA11" s="67" t="s">
+        <v>74</v>
+      </c>
+      <c r="AB11" s="51"/>
+      <c r="AC11" s="51" t="s">
+        <v>179</v>
+      </c>
+      <c r="AD11" s="67" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="12" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V12" s="67" t="s">
+        <v>130</v>
+      </c>
+      <c r="W12" s="67">
+        <v>7</v>
+      </c>
+      <c r="X12" s="67" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y12" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="Z12" s="67" t="s">
+        <v>11</v>
+      </c>
+      <c r="AA12" s="67" t="s">
+        <v>73</v>
+      </c>
+      <c r="AB12" s="51"/>
+      <c r="AC12" s="67" t="s">
+        <v>178</v>
+      </c>
+      <c r="AD12" s="67" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="13" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="V13" s="67" t="s">
+        <v>131</v>
+      </c>
+      <c r="W13" s="67">
+        <v>8</v>
+      </c>
+      <c r="X13" s="51"/>
+      <c r="Y13" s="67" t="s">
+        <v>25</v>
+      </c>
+      <c r="Z13" s="67" t="s">
+        <v>187</v>
+      </c>
+      <c r="AA13" s="51"/>
+      <c r="AB13" s="51"/>
+      <c r="AC13" s="67" t="s">
+        <v>185</v>
+      </c>
+      <c r="AD13" s="67" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="14" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I14" s="56"/>
+      <c r="J14" t="s">
+        <v>184</v>
+      </c>
+      <c r="R14" s="60"/>
+      <c r="S14" t="s">
+        <v>182</v>
+      </c>
+      <c r="V14" s="67" t="s">
+        <v>132</v>
+      </c>
+      <c r="W14" s="67">
+        <v>9</v>
+      </c>
+      <c r="X14" s="51"/>
+      <c r="Y14" s="67" t="s">
+        <v>15</v>
+      </c>
+      <c r="Z14" s="67" t="s">
+        <v>188</v>
+      </c>
+      <c r="AA14" s="51"/>
+      <c r="AB14" s="51"/>
+      <c r="AC14" s="51"/>
+      <c r="AD14" s="67" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="15" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I15" s="56"/>
+      <c r="J15" s="10" t="s">
+        <v>1</v>
+      </c>
+      <c r="K15" s="10" t="s">
+        <v>146</v>
+      </c>
+      <c r="L15" s="10" t="s">
+        <v>142</v>
+      </c>
+      <c r="M15" s="10" t="s">
+        <v>134</v>
+      </c>
+      <c r="N15" s="10" t="s">
+        <v>132</v>
+      </c>
+      <c r="R15" s="59"/>
+      <c r="S15" t="s">
+        <v>183</v>
+      </c>
+      <c r="V15" s="67" t="s">
+        <v>133</v>
+      </c>
+      <c r="W15" s="51"/>
+      <c r="X15" s="51"/>
+      <c r="Y15" s="67" t="s">
+        <v>31</v>
+      </c>
+      <c r="Z15" s="51"/>
+      <c r="AA15" s="51"/>
+      <c r="AB15" s="51"/>
+      <c r="AC15" s="51"/>
+      <c r="AD15" s="67" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="16" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I16" s="56"/>
+      <c r="J16" s="10" t="s">
+        <v>137</v>
+      </c>
+      <c r="K16" s="10" t="s">
+        <v>131</v>
+      </c>
+      <c r="L16" s="10" t="s">
+        <v>127</v>
+      </c>
+      <c r="M16" s="10" t="s">
+        <v>136</v>
+      </c>
+      <c r="N16" s="10" t="s">
+        <v>135</v>
+      </c>
+      <c r="V16" s="67" t="s">
+        <v>134</v>
+      </c>
+      <c r="W16" s="51"/>
+      <c r="X16" s="51"/>
+      <c r="Y16" s="67" t="s">
+        <v>14</v>
+      </c>
+      <c r="Z16" s="51"/>
+      <c r="AA16" s="51"/>
+      <c r="AB16" s="51"/>
+      <c r="AC16" s="51"/>
+      <c r="AD16" s="67" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="17" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I17" s="56"/>
+      <c r="J17" s="69" t="s">
+        <v>189</v>
+      </c>
+      <c r="K17" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="L17" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="M17" s="10" t="s">
+        <v>130</v>
+      </c>
+      <c r="N17" s="10" t="s">
+        <v>133</v>
+      </c>
+      <c r="V17" s="67" t="s">
+        <v>135</v>
+      </c>
+      <c r="W17" s="51"/>
+      <c r="X17" s="51"/>
+      <c r="Y17" s="68" t="s">
+        <v>30</v>
+      </c>
+      <c r="Z17" s="51"/>
+      <c r="AA17" s="51"/>
+      <c r="AB17" s="51"/>
+      <c r="AC17" s="51"/>
+      <c r="AD17" s="51"/>
+    </row>
+    <row r="18" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I18" s="56"/>
+      <c r="J18" s="57"/>
+      <c r="K18" s="57"/>
+      <c r="L18" s="57"/>
+      <c r="M18" s="58"/>
+      <c r="N18" s="70"/>
+      <c r="V18" s="67" t="s">
+        <v>136</v>
+      </c>
+      <c r="W18" s="51"/>
+      <c r="X18" s="51"/>
+      <c r="Y18" s="67" t="s">
+        <v>27</v>
+      </c>
+      <c r="Z18" s="51"/>
+      <c r="AA18" s="51"/>
+      <c r="AB18" s="51"/>
+      <c r="AC18" s="51"/>
+      <c r="AD18" s="51"/>
+    </row>
+    <row r="19" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I19" s="56"/>
+      <c r="V19" s="67" t="s">
+        <v>137</v>
+      </c>
+      <c r="W19" s="51"/>
+      <c r="X19" s="51"/>
+      <c r="Y19" s="51"/>
+      <c r="Z19" s="51"/>
+      <c r="AA19" s="51"/>
+      <c r="AB19" s="51"/>
+      <c r="AC19" s="51"/>
+      <c r="AD19" s="51"/>
+    </row>
+    <row r="20" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I20" s="56"/>
+      <c r="J20" s="56" t="s">
+        <v>149</v>
+      </c>
+      <c r="K20" s="56"/>
+      <c r="L20" s="56"/>
+      <c r="M20" s="56"/>
+      <c r="N20" s="56"/>
+      <c r="O20" s="56"/>
+      <c r="V20" s="67" t="s">
+        <v>138</v>
+      </c>
+      <c r="W20" s="51"/>
+      <c r="X20" s="51"/>
+      <c r="Y20" s="51"/>
+      <c r="Z20" s="51"/>
+      <c r="AA20" s="51"/>
+      <c r="AB20" s="51"/>
+      <c r="AC20" s="51"/>
+      <c r="AD20" s="51"/>
+    </row>
+    <row r="21" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I21" s="56"/>
+      <c r="J21" s="10" t="s">
+        <v>190</v>
+      </c>
+      <c r="K21" s="63"/>
+      <c r="L21" s="66" t="s">
+        <v>150</v>
+      </c>
+      <c r="M21" s="64" t="s">
+        <v>154</v>
+      </c>
+      <c r="N21" s="10" t="s">
+        <v>99</v>
+      </c>
+      <c r="O21" s="56"/>
+      <c r="V21" s="67" t="s">
+        <v>117</v>
+      </c>
+      <c r="W21" s="51"/>
+      <c r="X21" s="51"/>
+      <c r="Y21" s="51"/>
+      <c r="Z21" s="51"/>
+      <c r="AA21" s="51"/>
+      <c r="AB21" s="51"/>
+      <c r="AC21" s="51"/>
+      <c r="AD21" s="51"/>
+    </row>
+    <row r="22" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I22" s="56"/>
+      <c r="J22" s="11" t="s">
+        <v>191</v>
+      </c>
+      <c r="K22" s="66" t="s">
+        <v>153</v>
+      </c>
+      <c r="L22" s="65" t="s">
+        <v>151</v>
+      </c>
+      <c r="M22" s="66" t="s">
+        <v>152</v>
+      </c>
+      <c r="N22" s="62" t="s">
+        <v>156</v>
+      </c>
+      <c r="O22" s="56"/>
+      <c r="V22" s="67" t="s">
+        <v>139</v>
+      </c>
+      <c r="W22" s="51"/>
+      <c r="X22" s="51"/>
+      <c r="Y22" s="51"/>
+      <c r="Z22" s="51"/>
+      <c r="AA22" s="51"/>
+      <c r="AB22" s="51"/>
+      <c r="AC22" s="51"/>
+      <c r="AD22" s="51"/>
+    </row>
+    <row r="23" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I23" s="56"/>
+      <c r="J23" s="10" t="s">
+        <v>97</v>
+      </c>
+      <c r="K23" s="31" t="s">
+        <v>77</v>
+      </c>
+      <c r="L23" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M23" s="31" t="s">
+        <v>155</v>
+      </c>
+      <c r="N23" s="10" t="s">
+        <v>194</v>
+      </c>
+      <c r="O23" s="56"/>
+      <c r="V23" s="67" t="s">
+        <v>140</v>
+      </c>
+      <c r="W23" s="51"/>
+      <c r="X23" s="51"/>
+      <c r="Y23" s="51"/>
+      <c r="Z23" s="51"/>
+      <c r="AA23" s="51"/>
+      <c r="AB23" s="51"/>
+      <c r="AC23" s="51"/>
+      <c r="AD23" s="51"/>
+    </row>
+    <row r="24" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I24" s="56"/>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="57"/>
+      <c r="M24" s="58" t="s">
+        <v>96</v>
+      </c>
+      <c r="N24" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="O24" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="V24" s="67" t="s">
+        <v>141</v>
+      </c>
+      <c r="W24" s="51"/>
+      <c r="X24" s="51"/>
+      <c r="Y24" s="51"/>
+      <c r="Z24" s="51"/>
+      <c r="AA24" s="51"/>
+      <c r="AB24" s="51"/>
+      <c r="AC24" s="51"/>
+      <c r="AD24" s="51"/>
+    </row>
+    <row r="25" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I25" s="56"/>
+      <c r="J25" s="56"/>
+      <c r="K25" s="56"/>
+      <c r="L25" s="56"/>
+      <c r="M25" s="56"/>
+      <c r="N25" s="56"/>
+      <c r="O25" s="56"/>
+      <c r="V25" s="67" t="s">
+        <v>142</v>
+      </c>
+      <c r="W25" s="51"/>
+      <c r="X25" s="51"/>
+      <c r="Y25" s="51"/>
+      <c r="Z25" s="51"/>
+      <c r="AA25" s="51"/>
+      <c r="AB25" s="51"/>
+      <c r="AC25" s="51"/>
+      <c r="AD25" s="51"/>
+    </row>
+    <row r="26" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I26" s="56"/>
+      <c r="J26" s="56" t="s">
+        <v>157</v>
+      </c>
+      <c r="K26" s="56"/>
+      <c r="L26" s="56"/>
+      <c r="M26" s="56"/>
+      <c r="N26" s="56"/>
+      <c r="O26" s="56"/>
+      <c r="V26" s="67" t="s">
+        <v>143</v>
+      </c>
+      <c r="W26" s="51"/>
+      <c r="X26" s="51"/>
+      <c r="Y26" s="51"/>
+      <c r="Z26" s="51"/>
+      <c r="AA26" s="51"/>
+      <c r="AB26" s="51"/>
+      <c r="AC26" s="51"/>
+      <c r="AD26" s="51"/>
+    </row>
+    <row r="27" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I27" s="56"/>
+      <c r="J27" s="10"/>
+      <c r="K27" s="10">
+        <v>9</v>
+      </c>
+      <c r="L27" s="10">
+        <v>8</v>
+      </c>
+      <c r="M27" s="10">
+        <v>7</v>
+      </c>
+      <c r="N27" s="10" t="s">
+        <v>30</v>
+      </c>
+      <c r="O27" s="56"/>
+      <c r="V27" s="67" t="s">
+        <v>144</v>
+      </c>
+      <c r="W27" s="51"/>
+      <c r="X27" s="51"/>
+      <c r="Y27" s="51"/>
+      <c r="Z27" s="51"/>
+      <c r="AA27" s="51"/>
+      <c r="AB27" s="51"/>
+      <c r="AC27" s="51"/>
+      <c r="AD27" s="51"/>
+    </row>
+    <row r="28" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I28" s="56"/>
+      <c r="J28" s="10"/>
+      <c r="K28" s="10">
+        <v>6</v>
+      </c>
+      <c r="L28" s="10">
+        <v>5</v>
+      </c>
+      <c r="M28" s="10">
+        <v>4</v>
+      </c>
+      <c r="N28" s="10" t="s">
+        <v>4</v>
+      </c>
+      <c r="O28" s="56"/>
+      <c r="V28" s="67" t="s">
+        <v>145</v>
+      </c>
+      <c r="W28" s="51"/>
+      <c r="X28" s="51"/>
+      <c r="Y28" s="51"/>
+      <c r="Z28" s="51"/>
+      <c r="AA28" s="51"/>
+      <c r="AB28" s="51"/>
+      <c r="AC28" s="51"/>
+      <c r="AD28" s="51"/>
+    </row>
+    <row r="29" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="I29" s="56"/>
+      <c r="J29" s="61"/>
+      <c r="K29" s="10">
+        <v>3</v>
+      </c>
+      <c r="L29" s="10">
+        <v>2</v>
+      </c>
+      <c r="M29" s="10">
+        <v>1</v>
+      </c>
+      <c r="N29" s="10">
+        <v>0</v>
+      </c>
+      <c r="O29" s="56"/>
+      <c r="V29" s="67" t="s">
+        <v>146</v>
+      </c>
+      <c r="W29" s="51"/>
+      <c r="X29" s="51"/>
+      <c r="Y29" s="51"/>
+      <c r="Z29" s="51"/>
+      <c r="AA29" s="51"/>
+      <c r="AB29" s="51"/>
+      <c r="AC29" s="51"/>
+      <c r="AD29" s="51"/>
+    </row>
+    <row r="30" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A30" s="52"/>
+      <c r="I30" s="56"/>
+      <c r="J30" s="57"/>
+      <c r="K30" s="57"/>
+      <c r="L30" s="57"/>
+      <c r="M30" s="58" t="s">
+        <v>14</v>
+      </c>
+      <c r="N30" s="58" t="s">
+        <v>76</v>
+      </c>
+      <c r="O30" s="56" t="s">
+        <v>148</v>
+      </c>
+      <c r="V30" s="67" t="s">
+        <v>147</v>
+      </c>
+      <c r="W30" s="51"/>
+      <c r="X30" s="51"/>
+      <c r="Y30" s="51"/>
+      <c r="Z30" s="51"/>
+      <c r="AA30" s="51"/>
+      <c r="AB30" s="51"/>
+      <c r="AC30" s="51"/>
+      <c r="AD30" s="51"/>
+    </row>
+    <row r="31" spans="1:30" x14ac:dyDescent="0.25">
+      <c r="A31" s="52"/>
+      <c r="I31" s="56"/>
+      <c r="J31" s="56"/>
+      <c r="K31" s="56"/>
+      <c r="L31" s="56"/>
+      <c r="M31" s="56"/>
+      <c r="N31" s="56"/>
+      <c r="O31" s="56"/>
+      <c r="V31" s="51"/>
+      <c r="W31" s="51"/>
+      <c r="X31" s="51"/>
+      <c r="Y31" s="51"/>
+      <c r="Z31" s="51"/>
+      <c r="AA31" s="51"/>
+      <c r="AB31" s="51"/>
+      <c r="AC31" s="51"/>
+      <c r="AD31" s="51"/>
+    </row>
+    <row r="32" spans="1:30" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="I32" s="56"/>
+      <c r="J32" s="56" t="s">
+        <v>158</v>
+      </c>
+      <c r="K32" s="56"/>
+      <c r="L32" s="56"/>
+      <c r="M32" s="56"/>
+      <c r="N32" s="56"/>
+      <c r="O32" s="56"/>
+    </row>
+    <row r="33" spans="10:15" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="J33" s="71"/>
+      <c r="K33" s="72" t="s">
+        <v>66</v>
+      </c>
+      <c r="L33" s="72" t="s">
+        <v>65</v>
+      </c>
+      <c r="M33" s="73" t="s">
+        <v>64</v>
+      </c>
+      <c r="N33" s="62" t="s">
+        <v>69</v>
+      </c>
+      <c r="O33" s="56"/>
+    </row>
+    <row r="34" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J34" s="31"/>
+      <c r="K34" s="31" t="s">
+        <v>63</v>
+      </c>
+      <c r="L34" s="31" t="s">
+        <v>62</v>
+      </c>
+      <c r="M34" s="31" t="s">
+        <v>61</v>
+      </c>
+      <c r="N34" s="10" t="s">
+        <v>68</v>
+      </c>
+      <c r="O34" s="56"/>
+    </row>
+    <row r="35" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J35" s="10"/>
+      <c r="K35" s="10" t="s">
+        <v>60</v>
+      </c>
+      <c r="L35" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="M35" s="10" t="s">
+        <v>58</v>
+      </c>
+      <c r="N35" s="10" t="s">
+        <v>67</v>
+      </c>
+      <c r="O35" s="56"/>
+    </row>
+    <row r="36" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J36" s="57"/>
+      <c r="K36" s="57"/>
+      <c r="L36" s="57"/>
+      <c r="M36" s="58"/>
+      <c r="N36" s="58"/>
+      <c r="O36" s="56"/>
+    </row>
+    <row r="37" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="O37" s="56"/>
+    </row>
+    <row r="38" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J38" s="56" t="s">
+        <v>186</v>
+      </c>
+      <c r="K38" s="56"/>
+      <c r="L38" s="56"/>
+      <c r="M38" s="56"/>
+      <c r="N38" s="56"/>
+    </row>
+    <row r="39" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J39" s="61"/>
+      <c r="K39" s="10" t="s">
+        <v>10</v>
+      </c>
+      <c r="L39" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="M39" s="10" t="s">
+        <v>71</v>
+      </c>
+      <c r="N39" s="10" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="40" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J40" s="10"/>
+      <c r="K40" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="L40" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="M40" s="35" t="s">
+        <v>11</v>
+      </c>
+      <c r="N40" s="10" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J41" s="10"/>
+      <c r="K41" s="10" t="s">
+        <v>77</v>
+      </c>
+      <c r="L41" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="M41" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="N41" s="10" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="42" spans="10:15" x14ac:dyDescent="0.25">
+      <c r="J42" s="57"/>
+      <c r="K42" s="57"/>
+      <c r="L42" s="57"/>
+      <c r="M42" s="58"/>
+      <c r="N42" s="58" t="s">
+        <v>94</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="5" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
add lt for NAV
</commit_message>
<xml_diff>
--- a/Urchin Layouts.xlsx
+++ b/Urchin Layouts.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jhsch\Documents\Development\zmk-urchin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2299DEA-472A-4894-8B13-CC9596C321D6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CF7BD340-D561-49C2-AD90-8A9BA5443A79}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="1050" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
+    <workbookView xWindow="14295" yWindow="0" windowWidth="14610" windowHeight="15585" activeTab="1" xr2:uid="{4968A009-ADD2-40DC-B7CD-75D7443B6449}"/>
   </bookViews>
   <sheets>
     <sheet name="Layout" sheetId="9" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="374" uniqueCount="197">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="375" uniqueCount="198">
   <si>
     <t>esc</t>
   </si>
@@ -607,9 +607,6 @@
     <t>&gt;</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>ctl+w</t>
   </si>
   <si>
@@ -629,6 +626,12 @@
   </si>
   <si>
     <t xml:space="preserve">   </t>
+  </si>
+  <si>
+    <t>sft</t>
+  </si>
+  <si>
+    <t xml:space="preserve">' </t>
   </si>
 </sst>
 </file>
@@ -1128,7 +1131,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="22" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="77">
+  <cellXfs count="75">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center"/>
@@ -1327,25 +1330,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Heading 3" xfId="1" builtinId="18"/>
@@ -1703,45 +1700,45 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="70" t="s">
+      <c r="B2" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="N2" s="70" t="s">
+      <c r="C2" s="73"/>
+      <c r="D2" s="73"/>
+      <c r="E2" s="73"/>
+      <c r="F2" s="73"/>
+      <c r="G2" s="73"/>
+      <c r="H2" s="73"/>
+      <c r="I2" s="73"/>
+      <c r="J2" s="73"/>
+      <c r="K2" s="73"/>
+      <c r="L2" s="73"/>
+      <c r="N2" s="73" t="s">
         <v>82</v>
       </c>
-      <c r="O2" s="70"/>
-      <c r="P2" s="70"/>
-      <c r="Q2" s="70"/>
-      <c r="R2" s="70"/>
-      <c r="S2" s="70"/>
-      <c r="T2" s="70"/>
-      <c r="U2" s="70"/>
-      <c r="V2" s="70"/>
-      <c r="W2" s="70"/>
-      <c r="X2" s="70"/>
-      <c r="Z2" s="70" t="s">
+      <c r="O2" s="73"/>
+      <c r="P2" s="73"/>
+      <c r="Q2" s="73"/>
+      <c r="R2" s="73"/>
+      <c r="S2" s="73"/>
+      <c r="T2" s="73"/>
+      <c r="U2" s="73"/>
+      <c r="V2" s="73"/>
+      <c r="W2" s="73"/>
+      <c r="X2" s="73"/>
+      <c r="Z2" s="73" t="s">
         <v>83</v>
       </c>
-      <c r="AA2" s="70"/>
-      <c r="AB2" s="70"/>
-      <c r="AC2" s="70"/>
-      <c r="AD2" s="70"/>
-      <c r="AE2" s="70"/>
-      <c r="AF2" s="70"/>
-      <c r="AG2" s="70"/>
-      <c r="AH2" s="70"/>
-      <c r="AI2" s="70"/>
-      <c r="AJ2" s="70"/>
+      <c r="AA2" s="73"/>
+      <c r="AB2" s="73"/>
+      <c r="AC2" s="73"/>
+      <c r="AD2" s="73"/>
+      <c r="AE2" s="73"/>
+      <c r="AF2" s="73"/>
+      <c r="AG2" s="73"/>
+      <c r="AH2" s="73"/>
+      <c r="AI2" s="73"/>
+      <c r="AJ2" s="73"/>
     </row>
     <row r="3" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" s="4" t="s">
@@ -2047,45 +2044,45 @@
       <c r="E7" s="22"/>
     </row>
     <row r="8" spans="2:42" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B8" s="70" t="s">
+      <c r="B8" s="73" t="s">
         <v>100</v>
       </c>
-      <c r="C8" s="70"/>
-      <c r="D8" s="70"/>
-      <c r="E8" s="70"/>
-      <c r="F8" s="70"/>
-      <c r="G8" s="70"/>
-      <c r="H8" s="70"/>
-      <c r="I8" s="70"/>
-      <c r="J8" s="70"/>
-      <c r="K8" s="70"/>
-      <c r="L8" s="70"/>
-      <c r="N8" s="70" t="s">
+      <c r="C8" s="73"/>
+      <c r="D8" s="73"/>
+      <c r="E8" s="73"/>
+      <c r="F8" s="73"/>
+      <c r="G8" s="73"/>
+      <c r="H8" s="73"/>
+      <c r="I8" s="73"/>
+      <c r="J8" s="73"/>
+      <c r="K8" s="73"/>
+      <c r="L8" s="73"/>
+      <c r="N8" s="73" t="s">
         <v>84</v>
       </c>
-      <c r="O8" s="70"/>
-      <c r="P8" s="70"/>
-      <c r="Q8" s="70"/>
-      <c r="R8" s="70"/>
-      <c r="S8" s="70"/>
-      <c r="T8" s="70"/>
-      <c r="U8" s="70"/>
-      <c r="V8" s="70"/>
-      <c r="W8" s="70"/>
-      <c r="X8" s="70"/>
-      <c r="Z8" s="70" t="s">
+      <c r="O8" s="73"/>
+      <c r="P8" s="73"/>
+      <c r="Q8" s="73"/>
+      <c r="R8" s="73"/>
+      <c r="S8" s="73"/>
+      <c r="T8" s="73"/>
+      <c r="U8" s="73"/>
+      <c r="V8" s="73"/>
+      <c r="W8" s="73"/>
+      <c r="X8" s="73"/>
+      <c r="Z8" s="73" t="s">
         <v>101</v>
       </c>
-      <c r="AA8" s="70"/>
-      <c r="AB8" s="70"/>
-      <c r="AC8" s="70"/>
-      <c r="AD8" s="70"/>
-      <c r="AE8" s="70"/>
-      <c r="AF8" s="70"/>
-      <c r="AG8" s="70"/>
-      <c r="AH8" s="70"/>
-      <c r="AI8" s="70"/>
-      <c r="AJ8" s="70"/>
+      <c r="AA8" s="73"/>
+      <c r="AB8" s="73"/>
+      <c r="AC8" s="73"/>
+      <c r="AD8" s="73"/>
+      <c r="AE8" s="73"/>
+      <c r="AF8" s="73"/>
+      <c r="AG8" s="73"/>
+      <c r="AH8" s="73"/>
+      <c r="AI8" s="73"/>
+      <c r="AJ8" s="73"/>
     </row>
     <row r="9" spans="2:42" ht="30" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="48" t="s">
@@ -2360,19 +2357,19 @@
       <c r="B15" s="1" t="s">
         <v>106</v>
       </c>
-      <c r="N15" s="70" t="s">
+      <c r="N15" s="73" t="s">
         <v>81</v>
       </c>
-      <c r="O15" s="70"/>
-      <c r="P15" s="70"/>
-      <c r="Q15" s="70"/>
-      <c r="R15" s="70"/>
-      <c r="S15" s="70"/>
-      <c r="T15" s="70"/>
-      <c r="U15" s="70"/>
-      <c r="V15" s="70"/>
-      <c r="W15" s="70"/>
-      <c r="X15" s="70"/>
+      <c r="O15" s="73"/>
+      <c r="P15" s="73"/>
+      <c r="Q15" s="73"/>
+      <c r="R15" s="73"/>
+      <c r="S15" s="73"/>
+      <c r="T15" s="73"/>
+      <c r="U15" s="73"/>
+      <c r="V15" s="73"/>
+      <c r="W15" s="73"/>
+      <c r="X15" s="73"/>
       <c r="Z15"/>
       <c r="AA15"/>
       <c r="AB15"/>
@@ -2595,7 +2592,7 @@
   <dimension ref="A1:AI31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F15" sqref="F15"/>
+      <selection activeCell="R16" sqref="R16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2606,40 +2603,40 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A1" s="75"/>
-      <c r="B1" s="76" t="s">
+      <c r="A1" s="71"/>
+      <c r="B1" s="72" t="s">
         <v>120</v>
       </c>
-      <c r="C1" s="76" t="s">
+      <c r="C1" s="72" t="s">
         <v>118</v>
       </c>
-      <c r="D1" s="76" t="s">
+      <c r="D1" s="72" t="s">
         <v>119</v>
       </c>
-      <c r="E1" s="76" t="s">
+      <c r="E1" s="72" t="s">
         <v>121</v>
       </c>
-      <c r="F1" s="76" t="s">
+      <c r="F1" s="72" t="s">
         <v>122</v>
       </c>
     </row>
     <row r="2" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A2" s="75" t="s">
+      <c r="A2" s="71" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="76">
+      <c r="B2" s="72">
         <v>2</v>
       </c>
-      <c r="C2" s="76">
+      <c r="C2" s="72">
         <v>2</v>
       </c>
-      <c r="D2" s="76">
+      <c r="D2" s="72">
         <v>2</v>
       </c>
-      <c r="E2" s="76">
+      <c r="E2" s="72">
         <v>2</v>
       </c>
-      <c r="F2" s="76"/>
+      <c r="F2" s="72"/>
       <c r="J2" s="10">
         <v>1</v>
       </c>
@@ -2655,7 +2652,7 @@
       <c r="N2" s="10">
         <v>4</v>
       </c>
-      <c r="O2" s="71"/>
+      <c r="O2" s="8"/>
       <c r="P2" s="8"/>
       <c r="Q2" s="10">
         <v>4</v>
@@ -2674,20 +2671,20 @@
       </c>
     </row>
     <row r="3" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A3" s="75" t="s">
+      <c r="A3" s="71" t="s">
         <v>96</v>
       </c>
-      <c r="B3" s="76">
+      <c r="B3" s="72">
         <v>2</v>
       </c>
-      <c r="C3" s="76">
+      <c r="C3" s="72">
         <v>2</v>
       </c>
-      <c r="D3" s="76"/>
-      <c r="E3" s="76">
+      <c r="D3" s="72"/>
+      <c r="E3" s="72">
         <v>2</v>
       </c>
-      <c r="F3" s="76"/>
+      <c r="F3" s="72"/>
       <c r="J3" s="10">
         <v>2</v>
       </c>
@@ -2703,7 +2700,7 @@
       <c r="N3" s="10">
         <v>5</v>
       </c>
-      <c r="O3" s="71"/>
+      <c r="O3" s="8"/>
       <c r="P3" s="8"/>
       <c r="Q3" s="10">
         <v>5</v>
@@ -2721,45 +2718,45 @@
         <v>2</v>
       </c>
       <c r="AA3">
-        <f>COUNTA(Z5:Z32)</f>
+        <f t="shared" ref="AA3:AF3" si="0">COUNTA(Z5:Z32)</f>
         <v>0</v>
       </c>
       <c r="AB3">
-        <f>COUNTA(AA5:AA32)</f>
+        <f t="shared" si="0"/>
         <v>26</v>
       </c>
       <c r="AC3">
-        <f>COUNTA(AB5:AB32)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
       <c r="AD3">
-        <f>COUNTA(AC5:AC32)</f>
+        <f t="shared" si="0"/>
         <v>8</v>
       </c>
       <c r="AE3">
-        <f>COUNTA(AD5:AD32)</f>
+        <f t="shared" si="0"/>
         <v>14</v>
       </c>
       <c r="AF3">
-        <f>COUNTA(AE5:AE32)</f>
+        <f t="shared" si="0"/>
         <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:35" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="75" t="s">
+      <c r="A4" s="71" t="s">
         <v>94</v>
       </c>
-      <c r="B4" s="76"/>
-      <c r="C4" s="76">
+      <c r="B4" s="72"/>
+      <c r="C4" s="72">
         <v>2</v>
       </c>
-      <c r="D4" s="76">
+      <c r="D4" s="72">
         <v>2</v>
       </c>
-      <c r="E4" s="76">
+      <c r="E4" s="72">
         <v>2</v>
       </c>
-      <c r="F4" s="76"/>
+      <c r="F4" s="72"/>
       <c r="J4" s="10">
         <v>3</v>
       </c>
@@ -2775,7 +2772,7 @@
       <c r="N4" s="10">
         <v>6</v>
       </c>
-      <c r="O4" s="71"/>
+      <c r="O4" s="8"/>
       <c r="P4" s="8"/>
       <c r="Q4" s="10">
         <v>6</v>
@@ -2821,20 +2818,20 @@
       </c>
     </row>
     <row r="5" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A5" s="75" t="s">
+      <c r="A5" s="71" t="s">
         <v>97</v>
       </c>
-      <c r="B5" s="76">
+      <c r="B5" s="72">
         <v>2</v>
       </c>
-      <c r="C5" s="76">
+      <c r="C5" s="72">
         <v>2</v>
       </c>
-      <c r="D5" s="76">
+      <c r="D5" s="72">
         <v>2</v>
       </c>
-      <c r="E5" s="76"/>
-      <c r="F5" s="76"/>
+      <c r="E5" s="72"/>
+      <c r="F5" s="72"/>
       <c r="J5" s="8"/>
       <c r="K5" s="8"/>
       <c r="L5" s="8"/>
@@ -2844,7 +2841,7 @@
       <c r="N5" s="55">
         <v>1</v>
       </c>
-      <c r="O5" s="73"/>
+      <c r="O5" s="70"/>
       <c r="P5" s="8"/>
       <c r="Q5" s="10">
         <v>1</v>
@@ -2884,18 +2881,18 @@
       </c>
     </row>
     <row r="6" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A6" s="75" t="s">
-        <v>192</v>
-      </c>
-      <c r="B6" s="76">
+      <c r="A6" s="71" t="s">
+        <v>191</v>
+      </c>
+      <c r="B6" s="72">
         <v>1</v>
       </c>
-      <c r="C6" s="76">
+      <c r="C6" s="72">
         <v>1</v>
       </c>
-      <c r="D6" s="76"/>
-      <c r="E6" s="76"/>
-      <c r="F6" s="76"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="72"/>
+      <c r="F6" s="72"/>
       <c r="AA6" s="64" t="s">
         <v>124</v>
       </c>
@@ -2925,20 +2922,20 @@
       </c>
     </row>
     <row r="7" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A7" s="75" t="s">
-        <v>193</v>
-      </c>
-      <c r="B7" s="76"/>
-      <c r="C7" s="76">
+      <c r="A7" s="71" t="s">
+        <v>192</v>
+      </c>
+      <c r="B7" s="72"/>
+      <c r="C7" s="72">
         <v>2</v>
       </c>
-      <c r="D7" s="76">
+      <c r="D7" s="72">
         <v>2</v>
       </c>
-      <c r="E7" s="76">
+      <c r="E7" s="72">
         <v>5</v>
       </c>
-      <c r="F7" s="76"/>
+      <c r="F7" s="72"/>
       <c r="J7" t="s">
         <v>181</v>
       </c>
@@ -2971,18 +2968,18 @@
       </c>
     </row>
     <row r="8" spans="1:35" x14ac:dyDescent="0.25">
-      <c r="A8" s="75" t="s">
+      <c r="A8" s="71" t="s">
         <v>99</v>
       </c>
-      <c r="B8" s="76"/>
-      <c r="C8" s="76"/>
-      <c r="D8" s="76">
+      <c r="B8" s="72"/>
+      <c r="C8" s="72"/>
+      <c r="D8" s="72">
         <v>1</v>
       </c>
-      <c r="E8" s="76">
+      <c r="E8" s="72">
         <v>1</v>
       </c>
-      <c r="F8" s="76"/>
+      <c r="F8" s="72"/>
       <c r="J8" s="10" t="s">
         <v>117</v>
       </c>
@@ -2998,7 +2995,7 @@
       <c r="N8" s="10" t="s">
         <v>124</v>
       </c>
-      <c r="O8" s="71"/>
+      <c r="O8" s="8"/>
       <c r="P8" s="8"/>
       <c r="Q8" s="10" t="s">
         <v>132</v>
@@ -3059,7 +3056,7 @@
       <c r="N9" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="O9" s="71"/>
+      <c r="O9" s="8"/>
       <c r="P9" s="8"/>
       <c r="Q9" s="10" t="s">
         <v>135</v>
@@ -3118,7 +3115,7 @@
       <c r="N10" s="10" t="s">
         <v>143</v>
       </c>
-      <c r="O10" s="71"/>
+      <c r="O10" s="8"/>
       <c r="P10" s="8"/>
       <c r="Q10" s="10" t="s">
         <v>133</v>
@@ -3171,7 +3168,7 @@
       <c r="N11" s="55" t="s">
         <v>98</v>
       </c>
-      <c r="O11" s="73"/>
+      <c r="O11" s="70"/>
       <c r="P11" s="8"/>
       <c r="Q11" s="10"/>
       <c r="R11" s="55"/>
@@ -3264,7 +3261,7 @@
     </row>
     <row r="14" spans="1:35" x14ac:dyDescent="0.25">
       <c r="D14" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="AA14" s="64" t="s">
         <v>132</v>
@@ -3325,11 +3322,13 @@
       <c r="N16" s="10" t="s">
         <v>132</v>
       </c>
-      <c r="O16" s="71"/>
+      <c r="O16" s="8"/>
       <c r="Q16" s="10" t="s">
-        <v>190</v>
-      </c>
-      <c r="R16" s="60"/>
+        <v>189</v>
+      </c>
+      <c r="R16" s="60" t="s">
+        <v>76</v>
+      </c>
       <c r="S16" s="63" t="s">
         <v>150</v>
       </c>
@@ -3371,9 +3370,9 @@
       <c r="N17" s="10" t="s">
         <v>135</v>
       </c>
-      <c r="O17" s="71"/>
+      <c r="O17" s="8"/>
       <c r="Q17" s="11" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="R17" s="63" t="s">
         <v>153</v>
@@ -3403,7 +3402,7 @@
     </row>
     <row r="18" spans="1:35" x14ac:dyDescent="0.25">
       <c r="J18" s="35" t="s">
-        <v>189</v>
+        <v>197</v>
       </c>
       <c r="K18" s="10" t="s">
         <v>4</v>
@@ -3417,7 +3416,7 @@
       <c r="N18" s="10" t="s">
         <v>133</v>
       </c>
-      <c r="O18" s="71"/>
+      <c r="O18" s="8"/>
       <c r="Q18" s="10" t="s">
         <v>97</v>
       </c>
@@ -3431,10 +3430,7 @@
         <v>155</v>
       </c>
       <c r="U18" s="10" t="s">
-        <v>194</v>
-      </c>
-      <c r="V18" t="s">
-        <v>148</v>
+        <v>193</v>
       </c>
       <c r="AA18" s="64" t="s">
         <v>136</v>
@@ -3456,7 +3452,7 @@
       <c r="L19" s="8"/>
       <c r="M19" s="55"/>
       <c r="N19" s="66"/>
-      <c r="O19" s="72"/>
+      <c r="O19" s="70"/>
       <c r="Q19" s="8"/>
       <c r="R19" s="8"/>
       <c r="S19" s="8"/>
@@ -3464,7 +3460,10 @@
         <v>96</v>
       </c>
       <c r="U19" s="55" t="s">
-        <v>76</v>
+        <v>98</v>
+      </c>
+      <c r="V19" t="s">
+        <v>196</v>
       </c>
       <c r="AA19" s="64" t="s">
         <v>137</v>
@@ -3635,10 +3634,10 @@
       <c r="K25" s="8"/>
       <c r="L25" s="8"/>
       <c r="M25" s="55" t="s">
+        <v>76</v>
+      </c>
+      <c r="N25" s="74" t="s">
         <v>14</v>
-      </c>
-      <c r="N25" s="55" t="s">
-        <v>76</v>
       </c>
       <c r="Q25" s="8"/>
       <c r="R25" s="8"/>
@@ -3700,8 +3699,8 @@
       <c r="N28" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="Q28" s="74" t="s">
-        <v>195</v>
+      <c r="Q28" s="10" t="s">
+        <v>194</v>
       </c>
       <c r="R28" s="10"/>
       <c r="S28" s="10"/>

</xml_diff>